<commit_message>
AE-418 fix xlsx template by removing unnecessary formula
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -8536,9 +8536,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>249480</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>263160</xdr:rowOff>
+      <xdr:rowOff>262800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8552,7 +8552,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="759240" cy="215640"/>
+          <a:ext cx="758880" cy="215280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8573,9 +8573,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>149400</xdr:colOff>
+      <xdr:colOff>149040</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>263160</xdr:rowOff>
+      <xdr:rowOff>262800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8589,7 +8589,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1102320" cy="215640"/>
+          <a:ext cx="1101960" cy="215280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8610,9 +8610,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>22680</xdr:colOff>
+      <xdr:colOff>22320</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>264240</xdr:rowOff>
+      <xdr:rowOff>263880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8626,7 +8626,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1409400" cy="215640"/>
+          <a:ext cx="1409040" cy="215280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8647,9 +8647,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>346680</xdr:colOff>
+      <xdr:colOff>346320</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>264240</xdr:rowOff>
+      <xdr:rowOff>263880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8663,7 +8663,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1733400" cy="215640"/>
+          <a:ext cx="1733040" cy="215280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8684,9 +8684,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>219960</xdr:colOff>
+      <xdr:colOff>219600</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>277200</xdr:rowOff>
+      <xdr:rowOff>276840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8700,7 +8700,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2040480" cy="228600"/>
+          <a:ext cx="2040120" cy="228240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8721,9 +8721,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>163080</xdr:colOff>
+      <xdr:colOff>162720</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>264240</xdr:rowOff>
+      <xdr:rowOff>263880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8737,7 +8737,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2385360" cy="215640"/>
+          <a:ext cx="2385000" cy="215280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8758,9 +8758,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>103320</xdr:colOff>
+      <xdr:colOff>102960</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>263160</xdr:rowOff>
+      <xdr:rowOff>262800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8774,7 +8774,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2698560" cy="215640"/>
+          <a:ext cx="2698200" cy="215280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9174,9 +9174,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>319680</xdr:colOff>
+      <xdr:colOff>319320</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>80640</xdr:rowOff>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9186,7 +9186,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="7001640" cy="10064880"/>
+          <a:ext cx="7001280" cy="10064520"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9272,9 +9272,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>7560</xdr:colOff>
+      <xdr:colOff>7200</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>81720</xdr:rowOff>
+      <xdr:rowOff>81360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9284,7 +9284,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7018920" cy="268560"/>
+          <a:ext cx="7018560" cy="268200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9338,9 +9338,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>435960</xdr:colOff>
+      <xdr:colOff>435600</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>59040</xdr:rowOff>
+      <xdr:rowOff>58680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9350,7 +9350,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="797760" cy="269640"/>
+          <a:ext cx="797400" cy="269280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9402,9 +9402,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>434880</xdr:colOff>
+      <xdr:colOff>434520</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>198720</xdr:rowOff>
+      <xdr:rowOff>198360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9414,7 +9414,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="797760" cy="269640"/>
+          <a:ext cx="797400" cy="269280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9467,7 +9467,7 @@
   </sheetPr>
   <dimension ref="A1:AK262"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -19276,8 +19276,8 @@
   </sheetPr>
   <dimension ref="A1:AC82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19720,10 +19720,7 @@
       <c r="D14" s="113"/>
       <c r="E14" s="113"/>
       <c r="F14" s="14"/>
-      <c r="G14" s="114" t="str">
-        <f aca="false">IF(AND('4) E-luvun laskennan tulokset '!E18&lt;&gt;"*",'4) E-luvun laskennan tulokset '!E18&lt;&gt;0),'4) E-luvun laskennan tulokset '!E18,"")</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :kaukolampo]</v>
-      </c>
+      <c r="G14" s="114"/>
       <c r="H14" s="115" t="str">
         <f aca="false">IF(ISNUMBER(G14/'3) E-luvun laskennan lähtöt.'!$G$7),CEILING(G14/'3) E-luvun laskennan lähtöt.'!$G$7,1),"")</f>
         <v/>
@@ -22118,7 +22115,7 @@
   </sheetPr>
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
     </sheetView>
   </sheetViews>
@@ -24516,7 +24513,7 @@
   </sheetPr>
   <dimension ref="A1:T113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F77" activeCellId="0" sqref="F77"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
AE-420 add wrap text to large cells
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -4186,7 +4186,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
@@ -4866,7 +4866,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -19276,8 +19276,8 @@
   </sheetPr>
   <dimension ref="A1:AC82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24513,7 +24513,7 @@
   </sheetPr>
   <dimension ref="A1:T113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F77" activeCellId="0" sqref="F77"/>
     </sheetView>
   </sheetViews>
@@ -29003,8 +29003,8 @@
   </sheetPr>
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D57" activeCellId="0" sqref="D57"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30104,7 +30104,7 @@
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31025,7 +31025,7 @@
   </sheetPr>
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix various translation related template issues
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -3568,7 +3568,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="338">
+  <cellXfs count="339">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4907,6 +4907,10 @@
     </xf>
     <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -8536,9 +8540,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>249120</xdr:colOff>
+      <xdr:colOff>248760</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>262800</xdr:rowOff>
+      <xdr:rowOff>262440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8552,7 +8556,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="758880" cy="215280"/>
+          <a:ext cx="758520" cy="214920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8573,9 +8577,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>149040</xdr:colOff>
+      <xdr:colOff>148680</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>262800</xdr:rowOff>
+      <xdr:rowOff>262440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8589,7 +8593,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1101960" cy="215280"/>
+          <a:ext cx="1101600" cy="214920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8610,9 +8614,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>22320</xdr:colOff>
+      <xdr:colOff>21960</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>263880</xdr:rowOff>
+      <xdr:rowOff>263520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8626,7 +8630,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1409040" cy="215280"/>
+          <a:ext cx="1408680" cy="214920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8647,9 +8651,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>346320</xdr:colOff>
+      <xdr:colOff>345960</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>263880</xdr:rowOff>
+      <xdr:rowOff>263520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8663,7 +8667,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1733040" cy="215280"/>
+          <a:ext cx="1732680" cy="214920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8684,9 +8688,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>219600</xdr:colOff>
+      <xdr:colOff>219240</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>276840</xdr:rowOff>
+      <xdr:rowOff>276480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8700,7 +8704,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2040120" cy="228240"/>
+          <a:ext cx="2039760" cy="227880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8721,9 +8725,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>162720</xdr:colOff>
+      <xdr:colOff>162360</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>263880</xdr:rowOff>
+      <xdr:rowOff>263520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8737,7 +8741,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2385000" cy="215280"/>
+          <a:ext cx="2384640" cy="214920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8758,9 +8762,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>102960</xdr:colOff>
+      <xdr:colOff>102600</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>262800</xdr:rowOff>
+      <xdr:rowOff>262440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8774,7 +8778,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2698200" cy="215280"/>
+          <a:ext cx="2697840" cy="214920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9174,9 +9178,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>319320</xdr:colOff>
+      <xdr:colOff>318960</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9186,7 +9190,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="7001280" cy="10064520"/>
+          <a:ext cx="7000920" cy="10064160"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9272,9 +9276,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>7200</xdr:colOff>
+      <xdr:colOff>6840</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>81000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9284,7 +9288,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7018560" cy="268200"/>
+          <a:ext cx="7018200" cy="267840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9338,9 +9342,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>435600</xdr:colOff>
+      <xdr:colOff>435240</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>58680</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9350,7 +9354,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="797400" cy="269280"/>
+          <a:ext cx="797040" cy="268920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9402,9 +9406,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>434520</xdr:colOff>
+      <xdr:colOff>434160</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>198360</xdr:rowOff>
+      <xdr:rowOff>198000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9414,7 +9418,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="797400" cy="269280"/>
+          <a:ext cx="797040" cy="268920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -29003,8 +29007,8 @@
   </sheetPr>
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K64" activeCellId="0" sqref="K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29864,7 +29868,7 @@
         <f aca="false">A56</f>
         <v>[:huomiot :lammitys :toimenpide 1 :jaahdytys]</v>
       </c>
-      <c r="G63" s="0" t="str">
+      <c r="G63" s="335" t="str">
         <f aca="false">A57</f>
         <v>[:huomiot :lammitys :toimenpide 1 :eluvun-muutos]</v>
       </c>
@@ -30242,13 +30246,13 @@
       <c r="A13" s="150" t="s">
         <v>613</v>
       </c>
-      <c r="C13" s="335" t="s">
+      <c r="C13" s="336" t="s">
         <v>548</v>
       </c>
-      <c r="D13" s="335"/>
-      <c r="E13" s="335"/>
-      <c r="F13" s="335"/>
-      <c r="G13" s="335"/>
+      <c r="D13" s="336"/>
+      <c r="E13" s="336"/>
+      <c r="F13" s="336"/>
+      <c r="G13" s="336"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="150" t="s">
@@ -30257,13 +30261,13 @@
       <c r="C14" s="326" t="n">
         <v>1</v>
       </c>
-      <c r="D14" s="336" t="str">
+      <c r="D14" s="337" t="str">
         <f aca="false">A4</f>
         <v>[:huomiot :iv-ilmastointi :toimenpide 0 :nimi-fi]</v>
       </c>
-      <c r="E14" s="336"/>
-      <c r="F14" s="336"/>
-      <c r="G14" s="336"/>
+      <c r="E14" s="337"/>
+      <c r="F14" s="337"/>
+      <c r="G14" s="337"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="150" t="s">
@@ -30272,13 +30276,13 @@
       <c r="C15" s="326" t="n">
         <v>2</v>
       </c>
-      <c r="D15" s="336" t="str">
+      <c r="D15" s="337" t="str">
         <f aca="false">A6</f>
         <v>[:huomiot :iv-ilmastointi :toimenpide 1 :nimi-fi]</v>
       </c>
-      <c r="E15" s="336"/>
-      <c r="F15" s="336"/>
-      <c r="G15" s="336"/>
+      <c r="E15" s="337"/>
+      <c r="F15" s="337"/>
+      <c r="G15" s="337"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="150" t="s">
@@ -30287,13 +30291,13 @@
       <c r="C16" s="326" t="n">
         <v>3</v>
       </c>
-      <c r="D16" s="336" t="str">
+      <c r="D16" s="337" t="str">
         <f aca="false">A8</f>
         <v>[:huomiot :iv-ilmastointi :toimenpide 2 :nimi-fi]</v>
       </c>
-      <c r="E16" s="336"/>
-      <c r="F16" s="336"/>
-      <c r="G16" s="336"/>
+      <c r="E16" s="337"/>
+      <c r="F16" s="337"/>
+      <c r="G16" s="337"/>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="150" t="s">
@@ -30522,13 +30526,13 @@
       <c r="A33" s="150" t="s">
         <v>634</v>
       </c>
-      <c r="C33" s="335" t="s">
+      <c r="C33" s="336" t="s">
         <v>548</v>
       </c>
-      <c r="D33" s="335"/>
-      <c r="E33" s="335"/>
-      <c r="F33" s="335"/>
-      <c r="G33" s="335"/>
+      <c r="D33" s="336"/>
+      <c r="E33" s="336"/>
+      <c r="F33" s="336"/>
+      <c r="G33" s="336"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="150" t="s">
@@ -30537,13 +30541,13 @@
       <c r="C34" s="326" t="n">
         <v>1</v>
       </c>
-      <c r="D34" s="336" t="str">
+      <c r="D34" s="337" t="str">
         <f aca="false">A24</f>
         <v>[:huomiot :valaistus-muut :toimenpide 0 :nimi-fi]</v>
       </c>
-      <c r="E34" s="336"/>
-      <c r="F34" s="336"/>
-      <c r="G34" s="336"/>
+      <c r="E34" s="337"/>
+      <c r="F34" s="337"/>
+      <c r="G34" s="337"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="150" t="s">
@@ -30552,13 +30556,13 @@
       <c r="C35" s="326" t="n">
         <v>2</v>
       </c>
-      <c r="D35" s="336" t="str">
+      <c r="D35" s="337" t="str">
         <f aca="false">A26</f>
         <v>[:huomiot :valaistus-muut :toimenpide 1 :nimi-fi]</v>
       </c>
-      <c r="E35" s="336"/>
-      <c r="F35" s="336"/>
-      <c r="G35" s="336"/>
+      <c r="E35" s="337"/>
+      <c r="F35" s="337"/>
+      <c r="G35" s="337"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="150" t="s">
@@ -30567,13 +30571,13 @@
       <c r="C36" s="326" t="n">
         <v>3</v>
       </c>
-      <c r="D36" s="336" t="str">
+      <c r="D36" s="337" t="str">
         <f aca="false">A28</f>
         <v>[:huomiot :valaistus-muut :toimenpide 2 :nimi-fi]</v>
       </c>
-      <c r="E36" s="336"/>
-      <c r="F36" s="336"/>
-      <c r="G36" s="336"/>
+      <c r="E36" s="337"/>
+      <c r="F36" s="337"/>
+      <c r="G36" s="337"/>
     </row>
     <row r="37" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="150" t="s">
@@ -31025,7 +31029,7 @@
   </sheetPr>
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -31049,15 +31053,15 @@
       <c r="A2" s="150" t="s">
         <v>648</v>
       </c>
-      <c r="C2" s="337" t="s">
+      <c r="C2" s="338" t="s">
         <v>649</v>
       </c>
-      <c r="D2" s="337"/>
-      <c r="E2" s="337"/>
-      <c r="F2" s="337"/>
-      <c r="G2" s="337"/>
-      <c r="H2" s="337"/>
-      <c r="I2" s="337"/>
+      <c r="D2" s="338"/>
+      <c r="E2" s="338"/>
+      <c r="F2" s="338"/>
+      <c r="G2" s="338"/>
+      <c r="H2" s="338"/>
+      <c r="I2" s="338"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="318" t="s">

</xml_diff>

<commit_message>
AE-433 add huomiot.lisätiedot to pdf templates
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="653">
   <si>
     <t xml:space="preserve">[:id]</t>
   </si>
@@ -2894,6 +2894,12 @@
   </si>
   <si>
     <t xml:space="preserve">[:huomiot :suositukset-sv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:huomiot :lisatietoja-fi]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:huomiot :lisatietoja-sv]</t>
   </si>
   <si>
     <t xml:space="preserve">Lisätietoja energiatehokkuudesta</t>
@@ -3568,7 +3574,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="339">
+  <cellXfs count="340">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4919,6 +4925,10 @@
     </xf>
     <xf numFmtId="170" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -8540,9 +8550,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>248760</xdr:colOff>
+      <xdr:colOff>248400</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>262440</xdr:rowOff>
+      <xdr:rowOff>262080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8556,7 +8566,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="758520" cy="214920"/>
+          <a:ext cx="758160" cy="214560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8577,9 +8587,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>148680</xdr:colOff>
+      <xdr:colOff>148320</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>262440</xdr:rowOff>
+      <xdr:rowOff>262080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8593,7 +8603,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1101600" cy="214920"/>
+          <a:ext cx="1101240" cy="214560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8614,9 +8624,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>21960</xdr:colOff>
+      <xdr:colOff>21600</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>263520</xdr:rowOff>
+      <xdr:rowOff>263160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8630,7 +8640,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1408680" cy="214920"/>
+          <a:ext cx="1408320" cy="214560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8651,9 +8661,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>345960</xdr:colOff>
+      <xdr:colOff>345600</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>263520</xdr:rowOff>
+      <xdr:rowOff>263160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8667,7 +8677,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1732680" cy="214920"/>
+          <a:ext cx="1732320" cy="214560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8688,9 +8698,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>219240</xdr:colOff>
+      <xdr:colOff>218880</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>276480</xdr:rowOff>
+      <xdr:rowOff>276120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8704,7 +8714,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2039760" cy="227880"/>
+          <a:ext cx="2039400" cy="227520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8725,9 +8735,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>162360</xdr:colOff>
+      <xdr:colOff>162000</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>263520</xdr:rowOff>
+      <xdr:rowOff>263160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8741,7 +8751,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2384640" cy="214920"/>
+          <a:ext cx="2384280" cy="214560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8762,9 +8772,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>102600</xdr:colOff>
+      <xdr:colOff>102240</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>262440</xdr:rowOff>
+      <xdr:rowOff>262080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8778,7 +8788,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2697840" cy="214920"/>
+          <a:ext cx="2697480" cy="214560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9178,9 +9188,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>318960</xdr:colOff>
+      <xdr:colOff>318600</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>79920</xdr:rowOff>
+      <xdr:rowOff>79560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9190,7 +9200,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="7000920" cy="10064160"/>
+          <a:ext cx="7000560" cy="10063800"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9276,9 +9286,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
+      <xdr:colOff>6480</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>80640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9288,7 +9298,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7018200" cy="267840"/>
+          <a:ext cx="7017840" cy="267480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9342,9 +9352,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>435240</xdr:colOff>
+      <xdr:colOff>434880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>58320</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9354,7 +9364,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="797040" cy="268920"/>
+          <a:ext cx="796680" cy="268560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9406,9 +9416,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>434160</xdr:colOff>
+      <xdr:colOff>433800</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>198000</xdr:rowOff>
+      <xdr:rowOff>197640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9418,7 +9428,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="797040" cy="268920"/>
+          <a:ext cx="796680" cy="268560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -29007,7 +29017,7 @@
   </sheetPr>
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K64" activeCellId="0" sqref="K64"/>
     </sheetView>
   </sheetViews>
@@ -30107,8 +30117,8 @@
   </sheetPr>
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30713,7 +30723,9 @@
       <c r="G43" s="324"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="150"/>
+      <c r="A44" s="150" t="s">
+        <v>646</v>
+      </c>
       <c r="C44" s="324"/>
       <c r="D44" s="324"/>
       <c r="E44" s="324"/>
@@ -30721,7 +30733,9 @@
       <c r="G44" s="324"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="150"/>
+      <c r="A45" s="150" t="s">
+        <v>647</v>
+      </c>
       <c r="C45" s="324"/>
       <c r="D45" s="324"/>
       <c r="E45" s="324"/>
@@ -30826,7 +30840,7 @@
     </row>
     <row r="58" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C58" s="323" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="D58" s="94"/>
       <c r="E58" s="167"/>
@@ -30844,7 +30858,7 @@
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="150"/>
       <c r="C60" s="299" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="D60" s="299"/>
       <c r="E60" s="299"/>
@@ -30853,35 +30867,38 @@
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="150"/>
-      <c r="C61" s="307"/>
-      <c r="D61" s="307"/>
-      <c r="E61" s="307"/>
-      <c r="F61" s="307"/>
-      <c r="G61" s="307"/>
+      <c r="C61" s="338" t="str">
+        <f aca="false">A44</f>
+        <v>[:huomiot :lisatietoja-fi]</v>
+      </c>
+      <c r="D61" s="338"/>
+      <c r="E61" s="338"/>
+      <c r="F61" s="338"/>
+      <c r="G61" s="338"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="150"/>
-      <c r="C62" s="307"/>
-      <c r="D62" s="307"/>
-      <c r="E62" s="307"/>
-      <c r="F62" s="307"/>
-      <c r="G62" s="307"/>
+      <c r="C62" s="338"/>
+      <c r="D62" s="338"/>
+      <c r="E62" s="338"/>
+      <c r="F62" s="338"/>
+      <c r="G62" s="338"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="150"/>
-      <c r="C63" s="307"/>
-      <c r="D63" s="307"/>
-      <c r="E63" s="307"/>
-      <c r="F63" s="307"/>
-      <c r="G63" s="307"/>
+      <c r="C63" s="338"/>
+      <c r="D63" s="338"/>
+      <c r="E63" s="338"/>
+      <c r="F63" s="338"/>
+      <c r="G63" s="338"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="150"/>
-      <c r="C64" s="307"/>
-      <c r="D64" s="307"/>
-      <c r="E64" s="307"/>
-      <c r="F64" s="307"/>
-      <c r="G64" s="307"/>
+      <c r="C64" s="338"/>
+      <c r="D64" s="338"/>
+      <c r="E64" s="338"/>
+      <c r="F64" s="338"/>
+      <c r="G64" s="338"/>
     </row>
     <row r="65" customFormat="false" ht="5.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C65" s="143"/>
@@ -30892,7 +30909,7 @@
     </row>
     <row r="66" customFormat="false" ht="4.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="15">
     <mergeCell ref="C3:G12"/>
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="D14:G14"/>
@@ -30907,10 +30924,7 @@
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="C43:G57"/>
     <mergeCell ref="C60:G60"/>
-    <mergeCell ref="C61:G61"/>
-    <mergeCell ref="C62:G62"/>
-    <mergeCell ref="C63:G63"/>
-    <mergeCell ref="C64:G64"/>
+    <mergeCell ref="C61:G64"/>
   </mergeCells>
   <conditionalFormatting sqref="B15:D16 B13:C16 H13:AMJ17 B17 C45:C49 A65:AMJ1048576 A1:AMJ12 C42:G44 C57:G57 E59:AMJ59 A58:AMJ58 B59:B63 H60:AMJ64 C61:C63 B39:B57 H39:AMJ57 B19:B37 H19:AMJ37 C22:G22 C19:F21 D14">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="472">
@@ -31051,21 +31065,21 @@
     </row>
     <row r="2" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="150" t="s">
-        <v>648</v>
-      </c>
-      <c r="C2" s="338" t="s">
-        <v>649</v>
-      </c>
-      <c r="D2" s="338"/>
-      <c r="E2" s="338"/>
-      <c r="F2" s="338"/>
-      <c r="G2" s="338"/>
-      <c r="H2" s="338"/>
-      <c r="I2" s="338"/>
+        <v>650</v>
+      </c>
+      <c r="C2" s="339" t="s">
+        <v>651</v>
+      </c>
+      <c r="D2" s="339"/>
+      <c r="E2" s="339"/>
+      <c r="F2" s="339"/>
+      <c r="G2" s="339"/>
+      <c r="H2" s="339"/>
+      <c r="I2" s="339"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="318" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="C3" s="324" t="str">
         <f aca="false">A2</f>

</xml_diff>

<commit_message>
AE-435 fix lisatiedot field text wrap in pdf
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
@@ -4927,8 +4927,8 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -8550,9 +8550,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>248040</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>262080</xdr:rowOff>
+      <xdr:rowOff>261720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8566,7 +8566,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="758160" cy="214560"/>
+          <a:ext cx="757800" cy="214200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8587,9 +8587,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>148320</xdr:colOff>
+      <xdr:colOff>147960</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>262080</xdr:rowOff>
+      <xdr:rowOff>261720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8603,7 +8603,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1101240" cy="214560"/>
+          <a:ext cx="1100880" cy="214200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8624,9 +8624,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>21600</xdr:colOff>
+      <xdr:colOff>21240</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>263160</xdr:rowOff>
+      <xdr:rowOff>262800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8640,7 +8640,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1408320" cy="214560"/>
+          <a:ext cx="1407960" cy="214200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8661,9 +8661,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>345600</xdr:colOff>
+      <xdr:colOff>345240</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>263160</xdr:rowOff>
+      <xdr:rowOff>262800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8677,7 +8677,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1732320" cy="214560"/>
+          <a:ext cx="1731960" cy="214200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8698,9 +8698,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>218880</xdr:colOff>
+      <xdr:colOff>218520</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>276120</xdr:rowOff>
+      <xdr:rowOff>275760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8714,7 +8714,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2039400" cy="227520"/>
+          <a:ext cx="2039040" cy="227160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8735,9 +8735,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>161640</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>263160</xdr:rowOff>
+      <xdr:rowOff>262800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8751,7 +8751,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2384280" cy="214560"/>
+          <a:ext cx="2383920" cy="214200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8772,9 +8772,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>102240</xdr:colOff>
+      <xdr:colOff>101880</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>262080</xdr:rowOff>
+      <xdr:rowOff>261720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8788,7 +8788,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2697480" cy="214560"/>
+          <a:ext cx="2697120" cy="214200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9188,9 +9188,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>318600</xdr:colOff>
+      <xdr:colOff>318240</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>79560</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9200,7 +9200,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="7000560" cy="10063800"/>
+          <a:ext cx="7000200" cy="10063440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9286,9 +9286,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>6480</xdr:colOff>
+      <xdr:colOff>6120</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>80640</xdr:rowOff>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9298,7 +9298,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7017840" cy="267480"/>
+          <a:ext cx="7017480" cy="267120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9352,9 +9352,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>434880</xdr:colOff>
+      <xdr:colOff>434520</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>57960</xdr:rowOff>
+      <xdr:rowOff>57600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9364,7 +9364,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="796680" cy="268560"/>
+          <a:ext cx="796320" cy="268200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9416,9 +9416,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>433800</xdr:colOff>
+      <xdr:colOff>433440</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>197640</xdr:rowOff>
+      <xdr:rowOff>197280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9428,7 +9428,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="796680" cy="268560"/>
+          <a:ext cx="796320" cy="268200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -30118,7 +30118,7 @@
   <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
+      <selection pane="topLeft" activeCell="C61" activeCellId="0" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fix various bugs in xlsx templates
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="790">
   <si>
     <t xml:space="preserve">[:id]</t>
   </si>
@@ -62,7 +62,7 @@
     <t xml:space="preserve">[:perustiedot :katuosoite-sv]</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29169]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61210]</t>
   </si>
   <si>
     <t xml:space="preserve">[:perustiedot :rakennustunnus]</t>
@@ -80,31 +80,31 @@
     <t xml:space="preserve">[:perustiedot :alakayttotarkoitus-sv]</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29171]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29173]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29175]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29177]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61212]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61214]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61216]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61218]</t>
   </si>
   <si>
     <t xml:space="preserve">Rakennustunnus:</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29179]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61220]</t>
   </si>
   <si>
     <t xml:space="preserve">Rakennuksen valmistumisvuosi:</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29181]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29183]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61222]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61224]</t>
   </si>
   <si>
     <t xml:space="preserve">Rakennuksen käyttötarkoitusluokka:</t>
@@ -125,13 +125,13 @@
     <t xml:space="preserve">[:perustiedot :yritys :nimi]</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29186]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61227]</t>
   </si>
   <si>
     <t xml:space="preserve">             Energiatehokkuusluokka</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29188]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61230]</t>
   </si>
   <si>
     <t xml:space="preserve">Rakennuksen laskennallinen kokonaisenergiankulutus (E-luku)</t>
@@ -356,28 +356,28 @@
     <t xml:space="preserve">Muut sairaalat</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29190]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61234]</t>
   </si>
   <si>
     <t xml:space="preserve">YHTEENVETO RAKENNUKSEN ENERGIATEHOKKUUDESTA</t>
   </si>
   <si>
-    <t xml:space="preserve">[:lahtotiedot :lammitys :kuvaus-fi]</t>
+    <t xml:space="preserve">[:lahtotiedot :lammitys :label-fi]</t>
   </si>
   <si>
     <t xml:space="preserve">Laskettu kokonaisenergiankulutus ja ostoenergiankulutus</t>
   </si>
   <si>
-    <t xml:space="preserve">[:lahtotiedot :lammitys :kuvaus-sv]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:lahtotiedot :ilmanvaihto :kuvaus-fi]</t>
+    <t xml:space="preserve">[:lahtotiedot :lammitys :label-sv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :ilmanvaihto :label-fi]</t>
   </si>
   <si>
     <t xml:space="preserve">Lämmitetty nettoala</t>
   </si>
   <si>
-    <t xml:space="preserve">[:lahtotiedot :ilmanvaihto :kuvaus-sv]</t>
+    <t xml:space="preserve">[:lahtotiedot :ilmanvaihto :label-sv]</t>
   </si>
   <si>
     <t xml:space="preserve">Lämmitysjärjestelmän kuvaus</t>
@@ -645,25 +645,25 @@
     <t xml:space="preserve">[:tulokset :e-luokka-info :luokittelu :label-sv]</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29192]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29195]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29198]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29201]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29204]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29207]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29210]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61236]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61239]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61242]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61245]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61248]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61251]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61254]</t>
   </si>
   <si>
     <t xml:space="preserve">[:tulokset :e-luokka-info :e-luokka]</t>
@@ -1445,10 +1445,10 @@
     <t xml:space="preserve">[:lahtotiedot :lammitys :takka :tuotto]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:lahtotiedot :lammitys :ilmanlampopumppu :maara]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:lahtotiedot :lammitys :ilmanlampopumppu :tuotto]</t>
+    <t xml:space="preserve">[:lahtotiedot :lammitys :ilmalampopumppu :maara]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :lammitys :ilmalampopumppu :tuotto]</t>
   </si>
   <si>
     <t xml:space="preserve">[:lahtotiedot :jaahdytysjarjestelma :jaahdytyskauden-painotettu-kylmakerroin]</t>
@@ -1469,7 +1469,7 @@
     <t xml:space="preserve">Lämmitysenergian nettotarve</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29213]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61257]</t>
   </si>
   <si>
     <r>
@@ -1526,25 +1526,25 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29215]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29217]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29219]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29221]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61259]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61261]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61263]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61265]</t>
   </si>
   <si>
     <t xml:space="preserve">Sisäiset lämpökuormat eri käyttöasteilla</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29223]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29225]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61267]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61269]</t>
   </si>
   <si>
     <t xml:space="preserve">Käyttöaste</t>
@@ -1559,7 +1559,7 @@
     <t xml:space="preserve">Valaistus</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29227]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61271]</t>
   </si>
   <si>
     <r>
@@ -1585,16 +1585,16 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29229]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29231]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29233]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29235]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61273]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61275]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61277]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61279]</t>
   </si>
   <si>
     <t xml:space="preserve">E-LUVUN LASKENNAN TULOKSET</t>
@@ -2165,13 +2165,13 @@
     <t xml:space="preserve">[:tulokset :laskentatyokalu]</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29237]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61281]</t>
   </si>
   <si>
     <t xml:space="preserve">TOTEUTUNUT ENERGIANKULUTUS</t>
   </si>
   <si>
-    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--29239]</t>
+    <t xml:space="preserve">#function[solita.etp.service.energiatodistus-pdf/fn--61283]</t>
   </si>
   <si>
     <t xml:space="preserve">Saatavilla olevat ostoenergian määrät ilmoitetaan sellaisenaan ilman lämmöntarvelukukorjausta.</t>
@@ -2935,6 +2935,417 @@
   </si>
   <si>
     <t xml:space="preserve">[:lisamerkintoja-sv]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :rakennusvaippa :lampokapasiteetti]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :rakennusvaippa :ilmatilavuus]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :ilmanvaihto :tuloilma-lampotila]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :lammitys :tilat-ja-iv :lampopumppu-tuotto-osuus]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :lammitys :lammin-kayttovesi :lampopumppu-tuotto-osuus]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :lammitys :tilat-ja-iv :lampohavio-lammittamaton-tila]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:lahtotiedot :lammitys :lammin-kayttovesi :lampohavio-lammittamaton-tila]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 0 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 1 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 2 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 3 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 4 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 5 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 6 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 7 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 8 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 9 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 10 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 11 :hyoty :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :tuotto :aurinkosahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :tuotto :tuulisahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :tuotto :muusahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :tuotto :aurinkolampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :tuotto :muulampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :tuotto :lampopumppu]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :kulutus :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :kulutus :lampo]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :hyoty :sahko]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:tulokset :kuukausierittely 12 :hyoty :lampo]</t>
   </si>
 </sst>
 </file>
@@ -3574,7 +3985,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="340">
+  <cellXfs count="339">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4925,10 +5336,6 @@
     </xf>
     <xf numFmtId="170" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -8550,9 +8957,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>248040</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>261720</xdr:rowOff>
+      <xdr:rowOff>261000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8566,7 +8973,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="757800" cy="214200"/>
+          <a:ext cx="757080" cy="213480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8587,9 +8994,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>147960</xdr:colOff>
+      <xdr:colOff>147240</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>261720</xdr:rowOff>
+      <xdr:rowOff>261000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8603,7 +9010,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1100880" cy="214200"/>
+          <a:ext cx="1100160" cy="213480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8624,9 +9031,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>21240</xdr:colOff>
+      <xdr:colOff>20520</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>262800</xdr:rowOff>
+      <xdr:rowOff>262080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8640,7 +9047,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1407960" cy="214200"/>
+          <a:ext cx="1407240" cy="213480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8661,9 +9068,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>345240</xdr:colOff>
+      <xdr:colOff>344520</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>262800</xdr:rowOff>
+      <xdr:rowOff>262080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8677,7 +9084,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1731960" cy="214200"/>
+          <a:ext cx="1731240" cy="213480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8698,9 +9105,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>218520</xdr:colOff>
+      <xdr:colOff>217800</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>275760</xdr:rowOff>
+      <xdr:rowOff>275040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8714,7 +9121,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2039040" cy="227160"/>
+          <a:ext cx="2038320" cy="226440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8735,9 +9142,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>161640</xdr:colOff>
+      <xdr:colOff>160920</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>262800</xdr:rowOff>
+      <xdr:rowOff>262080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8751,7 +9158,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2383920" cy="214200"/>
+          <a:ext cx="2383200" cy="213480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8772,9 +9179,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>101880</xdr:colOff>
+      <xdr:colOff>101160</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>261720</xdr:rowOff>
+      <xdr:rowOff>261000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8788,7 +9195,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2697120" cy="214200"/>
+          <a:ext cx="2696400" cy="213480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9188,9 +9595,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>318240</xdr:colOff>
+      <xdr:colOff>317520</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9200,7 +9607,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="7000200" cy="10063440"/>
+          <a:ext cx="6999480" cy="10062720"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9286,9 +9693,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>6120</xdr:colOff>
+      <xdr:colOff>5400</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>79560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9298,7 +9705,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7017480" cy="267120"/>
+          <a:ext cx="7016760" cy="266400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9352,9 +9759,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>434520</xdr:colOff>
+      <xdr:colOff>433800</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:rowOff>56880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9364,7 +9771,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="796320" cy="268200"/>
+          <a:ext cx="795600" cy="267480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9416,9 +9823,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>433440</xdr:colOff>
+      <xdr:colOff>432720</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>197280</xdr:rowOff>
+      <xdr:rowOff>196560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9428,7 +9835,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="796320" cy="268200"/>
+          <a:ext cx="795600" cy="267480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9475,7 +9882,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
@@ -9879,7 +10286,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="16" t="str">
         <f aca="false">A5</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29169]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61210]</v>
       </c>
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
@@ -11325,7 +11732,7 @@
     <row r="48" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C48" s="79" t="str">
         <f aca="false">A21</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29186]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61227]</v>
       </c>
       <c r="D48" s="79"/>
       <c r="E48" s="79"/>
@@ -11337,7 +11744,7 @@
       <c r="K48" s="74"/>
       <c r="L48" s="80" t="str">
         <f aca="false">A22</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29188]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61230]</v>
       </c>
       <c r="M48" s="80"/>
       <c r="N48" s="80"/>
@@ -19284,7 +19691,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
@@ -19428,7 +19835,7 @@
       <c r="F5" s="14"/>
       <c r="G5" s="99" t="str">
         <f aca="false">A2</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29190]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61234]</v>
       </c>
       <c r="H5" s="29"/>
       <c r="I5" s="14"/>
@@ -19464,7 +19871,7 @@
       <c r="F6" s="14"/>
       <c r="G6" s="100" t="str">
         <f aca="false">A3</f>
-        <v>[:lahtotiedot :lammitys :kuvaus-fi]</v>
+        <v>[:lahtotiedot :lammitys :label-fi]</v>
       </c>
       <c r="H6" s="100"/>
       <c r="I6" s="100"/>
@@ -19500,7 +19907,7 @@
       <c r="F7" s="14"/>
       <c r="G7" s="101" t="str">
         <f aca="false">A5</f>
-        <v>[:lahtotiedot :ilmanvaihto :kuvaus-fi]</v>
+        <v>[:lahtotiedot :ilmanvaihto :label-fi]</v>
       </c>
       <c r="H7" s="101"/>
       <c r="I7" s="101"/>
@@ -20335,15 +20742,15 @@
       <c r="F29" s="14"/>
       <c r="H29" s="131" t="str">
         <f aca="false">A45</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29192]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61236]</v>
       </c>
       <c r="I29" s="132" t="str">
         <f aca="false">A46</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29195]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61239]</v>
       </c>
       <c r="J29" s="133" t="str">
         <f aca="false">A47</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29198]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61242]</v>
       </c>
       <c r="K29" s="129"/>
       <c r="M29" s="0"/>
@@ -20374,15 +20781,15 @@
       <c r="F30" s="14"/>
       <c r="H30" s="134" t="str">
         <f aca="false">A48</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29201]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61245]</v>
       </c>
       <c r="I30" s="135" t="str">
         <f aca="false">A49</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29204]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61248]</v>
       </c>
       <c r="J30" s="136" t="str">
         <f aca="false">A50</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29207]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61251]</v>
       </c>
       <c r="K30" s="129"/>
       <c r="M30" s="0"/>
@@ -20413,7 +20820,7 @@
       <c r="F31" s="14"/>
       <c r="H31" s="137" t="str">
         <f aca="false">A51</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29210]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61254]</v>
       </c>
       <c r="I31" s="138"/>
       <c r="J31" s="138"/>
@@ -22123,14 +22530,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M43" activeCellId="0" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22294,7 +22701,10 @@
       <c r="D11" s="173" t="s">
         <v>180</v>
       </c>
-      <c r="E11" s="179"/>
+      <c r="E11" s="179" t="str">
+        <f aca="false">A6</f>
+        <v>[:lahtotiedot :rakennusvaippa :ilmanvuotoluku]</v>
+      </c>
       <c r="F11" s="173"/>
       <c r="G11" s="170"/>
       <c r="H11" s="177"/>
@@ -22842,7 +23252,7 @@
       </c>
       <c r="E39" s="194" t="str">
         <f aca="false">A53</f>
-        <v>[:lahtotiedot :ilmanvaihto :kuvaus-fi]</v>
+        <v>[:lahtotiedot :ilmanvaihto :label-fi]</v>
       </c>
       <c r="F39" s="194"/>
       <c r="G39" s="194"/>
@@ -23084,7 +23494,7 @@
       </c>
       <c r="E53" s="194" t="str">
         <f aca="false">A64</f>
-        <v>[:lahtotiedot :lammitys :kuvaus-fi]</v>
+        <v>[:lahtotiedot :lammitys :label-fi]</v>
       </c>
       <c r="F53" s="194"/>
       <c r="G53" s="194"/>
@@ -23352,11 +23762,11 @@
       </c>
       <c r="E69" s="212" t="str">
         <f aca="false">A76</f>
-        <v>[:lahtotiedot :lammitys :ilmanlampopumppu :maara]</v>
+        <v>[:lahtotiedot :lammitys :ilmalampopumppu :maara]</v>
       </c>
       <c r="F69" s="212" t="str">
         <f aca="false">A77</f>
-        <v>[:lahtotiedot :lammitys :ilmanlampopumppu :tuotto]</v>
+        <v>[:lahtotiedot :lammitys :ilmalampopumppu :tuotto]</v>
       </c>
       <c r="G69" s="180"/>
       <c r="H69" s="177"/>
@@ -23662,19 +24072,19 @@
       <c r="D90" s="217"/>
       <c r="E90" s="197" t="str">
         <f aca="false">A81</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29213]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61257]</v>
       </c>
       <c r="F90" s="186" t="str">
         <f aca="false">A82</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29215]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61259]</v>
       </c>
       <c r="G90" s="186" t="str">
         <f aca="false">A83</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29217]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61261]</v>
       </c>
       <c r="H90" s="186" t="str">
         <f aca="false">A84</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29219]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61263]</v>
       </c>
       <c r="I90" s="175"/>
     </row>
@@ -23686,19 +24096,19 @@
       <c r="D91" s="217"/>
       <c r="E91" s="197" t="str">
         <f aca="false">A85</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29221]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61265]</v>
       </c>
       <c r="F91" s="186" t="str">
         <f aca="false">A86</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29223]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61267]</v>
       </c>
       <c r="G91" s="186" t="str">
         <f aca="false">A87</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29225]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61269]</v>
       </c>
       <c r="H91" s="186" t="str">
         <f aca="false">A88</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29227]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61271]</v>
       </c>
       <c r="I91" s="175"/>
     </row>
@@ -23710,19 +24120,19 @@
       <c r="D92" s="217"/>
       <c r="E92" s="197" t="str">
         <f aca="false">A89</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29229]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61273]</v>
       </c>
       <c r="F92" s="186" t="str">
         <f aca="false">A90</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29231]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61275]</v>
       </c>
       <c r="G92" s="186" t="str">
         <f aca="false">A91</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29233]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61277]</v>
       </c>
       <c r="H92" s="186" t="str">
         <f aca="false">A92</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29235]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61279]</v>
       </c>
       <c r="I92" s="175"/>
     </row>
@@ -24521,13 +24931,13 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:T113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F77" activeCellId="0" sqref="F77"/>
     </sheetView>
   </sheetViews>
@@ -27108,14 +27518,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:Y67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J51" activeCellId="0" sqref="J51"/>
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27219,7 +27629,7 @@
       <c r="C7" s="97"/>
       <c r="D7" s="61" t="str">
         <f aca="false">A2</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--29237]</v>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--61281]</v>
       </c>
       <c r="E7" s="14"/>
       <c r="G7" s="268"/>
@@ -29011,7 +29421,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
@@ -30111,13 +30521,13 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C61" activeCellId="0" sqref="C61"/>
     </sheetView>
   </sheetViews>
@@ -30867,38 +31277,38 @@
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="150"/>
-      <c r="C61" s="338" t="str">
+      <c r="C61" s="324" t="str">
         <f aca="false">A44</f>
         <v>[:huomiot :lisatietoja-fi]</v>
       </c>
-      <c r="D61" s="338"/>
-      <c r="E61" s="338"/>
-      <c r="F61" s="338"/>
-      <c r="G61" s="338"/>
+      <c r="D61" s="324"/>
+      <c r="E61" s="324"/>
+      <c r="F61" s="324"/>
+      <c r="G61" s="324"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="150"/>
-      <c r="C62" s="338"/>
-      <c r="D62" s="338"/>
-      <c r="E62" s="338"/>
-      <c r="F62" s="338"/>
-      <c r="G62" s="338"/>
+      <c r="C62" s="324"/>
+      <c r="D62" s="324"/>
+      <c r="E62" s="324"/>
+      <c r="F62" s="324"/>
+      <c r="G62" s="324"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="150"/>
-      <c r="C63" s="338"/>
-      <c r="D63" s="338"/>
-      <c r="E63" s="338"/>
-      <c r="F63" s="338"/>
-      <c r="G63" s="338"/>
+      <c r="C63" s="324"/>
+      <c r="D63" s="324"/>
+      <c r="E63" s="324"/>
+      <c r="F63" s="324"/>
+      <c r="G63" s="324"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="150"/>
-      <c r="C64" s="338"/>
-      <c r="D64" s="338"/>
-      <c r="E64" s="338"/>
-      <c r="F64" s="338"/>
-      <c r="G64" s="338"/>
+      <c r="C64" s="324"/>
+      <c r="D64" s="324"/>
+      <c r="E64" s="324"/>
+      <c r="F64" s="324"/>
+      <c r="G64" s="324"/>
     </row>
     <row r="65" customFormat="false" ht="5.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C65" s="143"/>
@@ -31037,11 +31447,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I140"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
@@ -31067,15 +31477,15 @@
       <c r="A2" s="150" t="s">
         <v>650</v>
       </c>
-      <c r="C2" s="339" t="s">
+      <c r="C2" s="338" t="s">
         <v>651</v>
       </c>
-      <c r="D2" s="339"/>
-      <c r="E2" s="339"/>
-      <c r="F2" s="339"/>
-      <c r="G2" s="339"/>
-      <c r="H2" s="339"/>
-      <c r="I2" s="339"/>
+      <c r="D2" s="338"/>
+      <c r="E2" s="338"/>
+      <c r="F2" s="338"/>
+      <c r="G2" s="338"/>
+      <c r="H2" s="338"/>
+      <c r="I2" s="338"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="318" t="s">
@@ -31093,6 +31503,9 @@
       <c r="I3" s="324"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="318" t="s">
+        <v>653</v>
+      </c>
       <c r="C4" s="324"/>
       <c r="D4" s="324"/>
       <c r="E4" s="324"/>
@@ -31102,6 +31515,9 @@
       <c r="I4" s="324"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="318" t="s">
+        <v>654</v>
+      </c>
       <c r="C5" s="324"/>
       <c r="D5" s="324"/>
       <c r="E5" s="324"/>
@@ -31111,6 +31527,9 @@
       <c r="I5" s="324"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="318" t="s">
+        <v>655</v>
+      </c>
       <c r="C6" s="324"/>
       <c r="D6" s="324"/>
       <c r="E6" s="324"/>
@@ -31120,6 +31539,9 @@
       <c r="I6" s="324"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="318" t="s">
+        <v>656</v>
+      </c>
       <c r="C7" s="324"/>
       <c r="D7" s="324"/>
       <c r="E7" s="324"/>
@@ -31129,6 +31551,9 @@
       <c r="I7" s="324"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="318" t="s">
+        <v>657</v>
+      </c>
       <c r="C8" s="324"/>
       <c r="D8" s="324"/>
       <c r="E8" s="324"/>
@@ -31138,6 +31563,9 @@
       <c r="I8" s="324"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="318" t="s">
+        <v>658</v>
+      </c>
       <c r="C9" s="324"/>
       <c r="D9" s="324"/>
       <c r="E9" s="324"/>
@@ -31147,6 +31575,9 @@
       <c r="I9" s="324"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="318" t="s">
+        <v>659</v>
+      </c>
       <c r="C10" s="324"/>
       <c r="D10" s="324"/>
       <c r="E10" s="324"/>
@@ -31156,6 +31587,9 @@
       <c r="I10" s="324"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="318" t="s">
+        <v>660</v>
+      </c>
       <c r="C11" s="324"/>
       <c r="D11" s="324"/>
       <c r="E11" s="324"/>
@@ -31165,6 +31599,9 @@
       <c r="I11" s="324"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="318" t="s">
+        <v>661</v>
+      </c>
       <c r="C12" s="324"/>
       <c r="D12" s="324"/>
       <c r="E12" s="324"/>
@@ -31174,6 +31611,9 @@
       <c r="I12" s="324"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="318" t="s">
+        <v>662</v>
+      </c>
       <c r="C13" s="324"/>
       <c r="D13" s="324"/>
       <c r="E13" s="324"/>
@@ -31183,6 +31623,9 @@
       <c r="I13" s="324"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="318" t="s">
+        <v>663</v>
+      </c>
       <c r="C14" s="324"/>
       <c r="D14" s="324"/>
       <c r="E14" s="324"/>
@@ -31192,6 +31635,9 @@
       <c r="I14" s="324"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="318" t="s">
+        <v>664</v>
+      </c>
       <c r="C15" s="324"/>
       <c r="D15" s="324"/>
       <c r="E15" s="324"/>
@@ -31201,6 +31647,9 @@
       <c r="I15" s="324"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="318" t="s">
+        <v>665</v>
+      </c>
       <c r="C16" s="324"/>
       <c r="D16" s="324"/>
       <c r="E16" s="324"/>
@@ -31210,6 +31659,9 @@
       <c r="I16" s="324"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="318" t="s">
+        <v>666</v>
+      </c>
       <c r="C17" s="324"/>
       <c r="D17" s="324"/>
       <c r="E17" s="324"/>
@@ -31219,6 +31671,9 @@
       <c r="I17" s="324"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="318" t="s">
+        <v>667</v>
+      </c>
       <c r="C18" s="324"/>
       <c r="D18" s="324"/>
       <c r="E18" s="324"/>
@@ -31228,6 +31683,9 @@
       <c r="I18" s="324"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="318" t="s">
+        <v>668</v>
+      </c>
       <c r="C19" s="324"/>
       <c r="D19" s="324"/>
       <c r="E19" s="324"/>
@@ -31237,6 +31695,9 @@
       <c r="I19" s="324"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="318" t="s">
+        <v>669</v>
+      </c>
       <c r="C20" s="324"/>
       <c r="D20" s="324"/>
       <c r="E20" s="324"/>
@@ -31246,6 +31707,9 @@
       <c r="I20" s="324"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="318" t="s">
+        <v>670</v>
+      </c>
       <c r="C21" s="324"/>
       <c r="D21" s="324"/>
       <c r="E21" s="324"/>
@@ -31255,6 +31719,9 @@
       <c r="I21" s="324"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="318" t="s">
+        <v>671</v>
+      </c>
       <c r="C22" s="324"/>
       <c r="D22" s="324"/>
       <c r="E22" s="324"/>
@@ -31264,6 +31731,9 @@
       <c r="I22" s="324"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="318" t="s">
+        <v>672</v>
+      </c>
       <c r="C23" s="324"/>
       <c r="D23" s="324"/>
       <c r="E23" s="324"/>
@@ -31273,6 +31743,9 @@
       <c r="I23" s="324"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="318" t="s">
+        <v>673</v>
+      </c>
       <c r="C24" s="324"/>
       <c r="D24" s="324"/>
       <c r="E24" s="324"/>
@@ -31282,6 +31755,9 @@
       <c r="I24" s="324"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="318" t="s">
+        <v>674</v>
+      </c>
       <c r="C25" s="324"/>
       <c r="D25" s="324"/>
       <c r="E25" s="324"/>
@@ -31291,6 +31767,9 @@
       <c r="I25" s="324"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="318" t="s">
+        <v>675</v>
+      </c>
       <c r="C26" s="324"/>
       <c r="D26" s="324"/>
       <c r="E26" s="324"/>
@@ -31300,6 +31779,9 @@
       <c r="I26" s="324"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="318" t="s">
+        <v>676</v>
+      </c>
       <c r="C27" s="324"/>
       <c r="D27" s="324"/>
       <c r="E27" s="324"/>
@@ -31309,6 +31791,9 @@
       <c r="I27" s="324"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="318" t="s">
+        <v>677</v>
+      </c>
       <c r="C28" s="324"/>
       <c r="D28" s="324"/>
       <c r="E28" s="324"/>
@@ -31318,6 +31803,9 @@
       <c r="I28" s="324"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="318" t="s">
+        <v>678</v>
+      </c>
       <c r="C29" s="324"/>
       <c r="D29" s="324"/>
       <c r="E29" s="324"/>
@@ -31327,6 +31815,9 @@
       <c r="I29" s="324"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="318" t="s">
+        <v>679</v>
+      </c>
       <c r="C30" s="324"/>
       <c r="D30" s="324"/>
       <c r="E30" s="324"/>
@@ -31336,6 +31827,9 @@
       <c r="I30" s="324"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="318" t="s">
+        <v>680</v>
+      </c>
       <c r="C31" s="324"/>
       <c r="D31" s="324"/>
       <c r="E31" s="324"/>
@@ -31345,6 +31839,9 @@
       <c r="I31" s="324"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="318" t="s">
+        <v>681</v>
+      </c>
       <c r="C32" s="324"/>
       <c r="D32" s="324"/>
       <c r="E32" s="324"/>
@@ -31354,6 +31851,9 @@
       <c r="I32" s="324"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="318" t="s">
+        <v>682</v>
+      </c>
       <c r="C33" s="324"/>
       <c r="D33" s="324"/>
       <c r="E33" s="324"/>
@@ -31363,6 +31863,9 @@
       <c r="I33" s="324"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="318" t="s">
+        <v>683</v>
+      </c>
       <c r="C34" s="324"/>
       <c r="D34" s="324"/>
       <c r="E34" s="324"/>
@@ -31372,6 +31875,9 @@
       <c r="I34" s="324"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="318" t="s">
+        <v>684</v>
+      </c>
       <c r="C35" s="324"/>
       <c r="D35" s="324"/>
       <c r="E35" s="324"/>
@@ -31381,6 +31887,9 @@
       <c r="I35" s="324"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="318" t="s">
+        <v>685</v>
+      </c>
       <c r="C36" s="324"/>
       <c r="D36" s="324"/>
       <c r="E36" s="324"/>
@@ -31390,6 +31899,9 @@
       <c r="I36" s="324"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="318" t="s">
+        <v>686</v>
+      </c>
       <c r="C37" s="324"/>
       <c r="D37" s="324"/>
       <c r="E37" s="324"/>
@@ -31399,6 +31911,9 @@
       <c r="I37" s="324"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="318" t="s">
+        <v>687</v>
+      </c>
       <c r="C38" s="324"/>
       <c r="D38" s="324"/>
       <c r="E38" s="324"/>
@@ -31408,6 +31923,9 @@
       <c r="I38" s="324"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="318" t="s">
+        <v>688</v>
+      </c>
       <c r="C39" s="324"/>
       <c r="D39" s="324"/>
       <c r="E39" s="324"/>
@@ -31417,6 +31935,9 @@
       <c r="I39" s="324"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="318" t="s">
+        <v>689</v>
+      </c>
       <c r="C40" s="324"/>
       <c r="D40" s="324"/>
       <c r="E40" s="324"/>
@@ -31426,6 +31947,9 @@
       <c r="I40" s="324"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="318" t="s">
+        <v>690</v>
+      </c>
       <c r="C41" s="324"/>
       <c r="D41" s="324"/>
       <c r="E41" s="324"/>
@@ -31435,6 +31959,9 @@
       <c r="I41" s="324"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="318" t="s">
+        <v>691</v>
+      </c>
       <c r="C42" s="324"/>
       <c r="D42" s="324"/>
       <c r="E42" s="324"/>
@@ -31444,6 +31971,9 @@
       <c r="I42" s="324"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="318" t="s">
+        <v>692</v>
+      </c>
       <c r="C43" s="324"/>
       <c r="D43" s="324"/>
       <c r="E43" s="324"/>
@@ -31453,6 +31983,9 @@
       <c r="I43" s="324"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="318" t="s">
+        <v>693</v>
+      </c>
       <c r="C44" s="324"/>
       <c r="D44" s="324"/>
       <c r="E44" s="324"/>
@@ -31462,6 +31995,9 @@
       <c r="I44" s="324"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="318" t="s">
+        <v>694</v>
+      </c>
       <c r="C45" s="324"/>
       <c r="D45" s="324"/>
       <c r="E45" s="324"/>
@@ -31471,6 +32007,9 @@
       <c r="I45" s="324"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="318" t="s">
+        <v>695</v>
+      </c>
       <c r="C46" s="324"/>
       <c r="D46" s="324"/>
       <c r="E46" s="324"/>
@@ -31480,6 +32019,9 @@
       <c r="I46" s="324"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="318" t="s">
+        <v>696</v>
+      </c>
       <c r="C47" s="324"/>
       <c r="D47" s="324"/>
       <c r="E47" s="324"/>
@@ -31489,6 +32031,9 @@
       <c r="I47" s="324"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="318" t="s">
+        <v>697</v>
+      </c>
       <c r="C48" s="324"/>
       <c r="D48" s="324"/>
       <c r="E48" s="324"/>
@@ -31498,6 +32043,9 @@
       <c r="I48" s="324"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="318" t="s">
+        <v>698</v>
+      </c>
       <c r="C49" s="324"/>
       <c r="D49" s="324"/>
       <c r="E49" s="324"/>
@@ -31507,6 +32055,9 @@
       <c r="I49" s="324"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="318" t="s">
+        <v>699</v>
+      </c>
       <c r="C50" s="324"/>
       <c r="D50" s="324"/>
       <c r="E50" s="324"/>
@@ -31516,6 +32067,9 @@
       <c r="I50" s="324"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="318" t="s">
+        <v>700</v>
+      </c>
       <c r="C51" s="324"/>
       <c r="D51" s="324"/>
       <c r="E51" s="324"/>
@@ -31525,6 +32079,9 @@
       <c r="I51" s="324"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="318" t="s">
+        <v>701</v>
+      </c>
       <c r="C52" s="324"/>
       <c r="D52" s="324"/>
       <c r="E52" s="324"/>
@@ -31534,6 +32091,9 @@
       <c r="I52" s="324"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="318" t="s">
+        <v>702</v>
+      </c>
       <c r="C53" s="324"/>
       <c r="D53" s="324"/>
       <c r="E53" s="324"/>
@@ -31543,6 +32103,9 @@
       <c r="I53" s="324"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="318" t="s">
+        <v>703</v>
+      </c>
       <c r="C54" s="324"/>
       <c r="D54" s="324"/>
       <c r="E54" s="324"/>
@@ -31552,6 +32115,9 @@
       <c r="I54" s="324"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="318" t="s">
+        <v>704</v>
+      </c>
       <c r="C55" s="324"/>
       <c r="D55" s="324"/>
       <c r="E55" s="324"/>
@@ -31561,6 +32127,9 @@
       <c r="I55" s="324"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="318" t="s">
+        <v>705</v>
+      </c>
       <c r="C56" s="324"/>
       <c r="D56" s="324"/>
       <c r="E56" s="324"/>
@@ -31570,6 +32139,9 @@
       <c r="I56" s="324"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="318" t="s">
+        <v>706</v>
+      </c>
       <c r="C57" s="324"/>
       <c r="D57" s="324"/>
       <c r="E57" s="324"/>
@@ -31579,6 +32151,9 @@
       <c r="I57" s="324"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="318" t="s">
+        <v>707</v>
+      </c>
       <c r="C58" s="324"/>
       <c r="D58" s="324"/>
       <c r="E58" s="324"/>
@@ -31588,6 +32163,9 @@
       <c r="I58" s="324"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="318" t="s">
+        <v>708</v>
+      </c>
       <c r="C59" s="324"/>
       <c r="D59" s="324"/>
       <c r="E59" s="324"/>
@@ -31597,6 +32175,9 @@
       <c r="I59" s="324"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="318" t="s">
+        <v>709</v>
+      </c>
       <c r="C60" s="324"/>
       <c r="D60" s="324"/>
       <c r="E60" s="324"/>
@@ -31606,6 +32187,9 @@
       <c r="I60" s="324"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="318" t="s">
+        <v>710</v>
+      </c>
       <c r="C61" s="324"/>
       <c r="D61" s="324"/>
       <c r="E61" s="324"/>
@@ -31615,6 +32199,9 @@
       <c r="I61" s="324"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="318" t="s">
+        <v>711</v>
+      </c>
       <c r="C62" s="324"/>
       <c r="D62" s="324"/>
       <c r="E62" s="324"/>
@@ -31624,6 +32211,9 @@
       <c r="I62" s="324"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="318" t="s">
+        <v>712</v>
+      </c>
       <c r="C63" s="324"/>
       <c r="D63" s="324"/>
       <c r="E63" s="324"/>
@@ -31633,6 +32223,9 @@
       <c r="I63" s="324"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="318" t="s">
+        <v>713</v>
+      </c>
       <c r="C64" s="324"/>
       <c r="D64" s="324"/>
       <c r="E64" s="324"/>
@@ -31642,6 +32235,9 @@
       <c r="I64" s="324"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="318" t="s">
+        <v>714</v>
+      </c>
       <c r="C65" s="324"/>
       <c r="D65" s="324"/>
       <c r="E65" s="324"/>
@@ -31651,6 +32247,9 @@
       <c r="I65" s="324"/>
     </row>
     <row r="66" customFormat="false" ht="5.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="318" t="s">
+        <v>715</v>
+      </c>
       <c r="C66" s="143"/>
       <c r="D66" s="144"/>
       <c r="E66" s="144"/>
@@ -31659,7 +32258,376 @@
       <c r="H66" s="144"/>
       <c r="I66" s="157"/>
     </row>
-    <row r="67" customFormat="false" ht="4.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="4.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="318" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="318" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="318" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="318" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="318" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="318" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="318" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="318" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="318" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="318" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="318" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="318" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="318" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="318" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="318" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="318" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="318" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="318" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="318" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="318" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="318" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="318" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="318" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="318" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="318" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="318" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="318" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="318" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="318" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="318" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="318" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="318" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="318" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="318" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="318" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="318" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="318" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="318" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="318" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="318" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="318" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="318" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="318" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="318" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="318" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="318" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="318" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="318" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="318" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="318" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="318" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="318" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="318" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="318" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="318" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="318" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="318" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="318" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="318" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="318" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="318" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="318" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="318" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="318" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="318" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="318" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="318" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="318" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="318" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="318" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="318" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="318" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="318" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="318" t="s">
+        <v>789</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C2:I2"/>

</xml_diff>

<commit_message>
Fix bug in pdf creation where zeroes were inserted in case of empty strings and nils
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
@@ -8957,9 +8957,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246960</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>261000</xdr:rowOff>
+      <xdr:rowOff>260640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8973,7 +8973,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="757080" cy="213480"/>
+          <a:ext cx="756720" cy="213120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8994,9 +8994,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>147240</xdr:colOff>
+      <xdr:colOff>146880</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>261000</xdr:rowOff>
+      <xdr:rowOff>260640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9010,7 +9010,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1100160" cy="213480"/>
+          <a:ext cx="1099800" cy="213120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9031,9 +9031,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>20520</xdr:colOff>
+      <xdr:colOff>20160</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>262080</xdr:rowOff>
+      <xdr:rowOff>261720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9047,7 +9047,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1407240" cy="213480"/>
+          <a:ext cx="1406880" cy="213120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9068,9 +9068,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>344520</xdr:colOff>
+      <xdr:colOff>344160</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>262080</xdr:rowOff>
+      <xdr:rowOff>261720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9084,7 +9084,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1731240" cy="213480"/>
+          <a:ext cx="1730880" cy="213120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9105,9 +9105,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>217800</xdr:colOff>
+      <xdr:colOff>217440</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>275040</xdr:rowOff>
+      <xdr:rowOff>274680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9121,7 +9121,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2038320" cy="226440"/>
+          <a:ext cx="2037960" cy="226080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9142,9 +9142,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>160920</xdr:colOff>
+      <xdr:colOff>160560</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>262080</xdr:rowOff>
+      <xdr:rowOff>261720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9158,7 +9158,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2383200" cy="213480"/>
+          <a:ext cx="2382840" cy="213120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9179,9 +9179,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>101160</xdr:colOff>
+      <xdr:colOff>100800</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>261000</xdr:rowOff>
+      <xdr:rowOff>260640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9195,7 +9195,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2696400" cy="213480"/>
+          <a:ext cx="2696040" cy="213120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9595,9 +9595,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>317520</xdr:colOff>
+      <xdr:colOff>317160</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9607,7 +9607,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="6999480" cy="10062720"/>
+          <a:ext cx="6999120" cy="10062360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9693,9 +9693,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>5400</xdr:colOff>
+      <xdr:colOff>5040</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>79560</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9705,7 +9705,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7016760" cy="266400"/>
+          <a:ext cx="7016400" cy="266040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9759,9 +9759,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>433800</xdr:colOff>
+      <xdr:colOff>433440</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9771,7 +9771,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="795600" cy="267480"/>
+          <a:ext cx="795240" cy="267120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9823,9 +9823,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>432720</xdr:colOff>
+      <xdr:colOff>432360</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>196560</xdr:rowOff>
+      <xdr:rowOff>196200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9835,7 +9835,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="795600" cy="267480"/>
+          <a:ext cx="795240" cy="267120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -22536,8 +22536,8 @@
   </sheetPr>
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M43" activeCellId="0" sqref="M43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H60" activeCellId="0" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Implement various fixes to xlsx templates
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -2199,6 +2199,7 @@
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">m</t>
     </r>
@@ -2210,6 +2211,7 @@
         <color rgb="FF009EE0"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -3388,7 +3390,7 @@
     <numFmt numFmtId="173" formatCode="#,##0.00"/>
     <numFmt numFmtId="174" formatCode="0.0"/>
   </numFmts>
-  <fonts count="40">
+  <fonts count="38">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3641,21 +3643,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF009EE0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <vertAlign val="superscript"/>
-      <sz val="10"/>
-      <color rgb="FF009EE0"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4584,7 +4571,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4880,15 +4867,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5096,7 +5083,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5124,7 +5111,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5216,7 +5203,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5292,11 +5279,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8992,9 +8979,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>246600</xdr:colOff>
+      <xdr:colOff>246240</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>260280</xdr:rowOff>
+      <xdr:rowOff>259920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9008,7 +8995,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="756360" cy="212760"/>
+          <a:ext cx="756000" cy="212400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9029,9 +9016,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>146520</xdr:colOff>
+      <xdr:colOff>146160</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>260280</xdr:rowOff>
+      <xdr:rowOff>259920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9045,7 +9032,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1099440" cy="212760"/>
+          <a:ext cx="1099080" cy="212400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9066,9 +9053,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>19800</xdr:colOff>
+      <xdr:colOff>19440</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>261360</xdr:rowOff>
+      <xdr:rowOff>261000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9082,7 +9069,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1406520" cy="212760"/>
+          <a:ext cx="1406160" cy="212400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9103,9 +9090,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>343800</xdr:colOff>
+      <xdr:colOff>343440</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>261360</xdr:rowOff>
+      <xdr:rowOff>261000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9119,7 +9106,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1730520" cy="212760"/>
+          <a:ext cx="1730160" cy="212400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9140,9 +9127,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>217080</xdr:colOff>
+      <xdr:colOff>216720</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>274320</xdr:rowOff>
+      <xdr:rowOff>273960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9156,7 +9143,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2037600" cy="225720"/>
+          <a:ext cx="2037240" cy="225360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9177,9 +9164,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>160200</xdr:colOff>
+      <xdr:colOff>159840</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>261360</xdr:rowOff>
+      <xdr:rowOff>261000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9193,7 +9180,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2382480" cy="212760"/>
+          <a:ext cx="2382120" cy="212400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9214,9 +9201,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>100440</xdr:colOff>
+      <xdr:colOff>100080</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>260280</xdr:rowOff>
+      <xdr:rowOff>259920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9230,7 +9217,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2695680" cy="212760"/>
+          <a:ext cx="2695320" cy="212400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9630,9 +9617,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>316800</xdr:colOff>
+      <xdr:colOff>316440</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>77760</xdr:rowOff>
+      <xdr:rowOff>77400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9642,7 +9629,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="6998760" cy="10062000"/>
+          <a:ext cx="6998400" cy="10061640"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9728,9 +9715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>4680</xdr:colOff>
+      <xdr:colOff>4320</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9740,7 +9727,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7016040" cy="265680"/>
+          <a:ext cx="7015680" cy="265320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9794,9 +9781,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>433080</xdr:colOff>
+      <xdr:colOff>432720</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>56160</xdr:rowOff>
+      <xdr:rowOff>55800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9806,7 +9793,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="794880" cy="266760"/>
+          <a:ext cx="794520" cy="266400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9858,9 +9845,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>432000</xdr:colOff>
+      <xdr:colOff>431640</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>195840</xdr:rowOff>
+      <xdr:rowOff>195480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9870,7 +9857,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="794880" cy="266760"/>
+          <a:ext cx="794520" cy="266400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -19733,7 +19720,7 @@
   <dimension ref="A1:AC82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
+      <selection pane="topLeft" activeCell="L20" activeCellId="0" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22572,7 +22559,7 @@
   <dimension ref="A1:N94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H60" activeCellId="0" sqref="H60"/>
+      <selection pane="topLeft" activeCell="M79" activeCellId="0" sqref="M79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23855,8 +23842,8 @@
       <c r="E73" s="213" t="s">
         <v>296</v>
       </c>
-      <c r="F73" s="180"/>
-      <c r="G73" s="180"/>
+      <c r="F73" s="214"/>
+      <c r="G73" s="214"/>
       <c r="H73" s="177"/>
       <c r="I73" s="175"/>
     </row>
@@ -23869,8 +23856,8 @@
       <c r="E74" s="183" t="s">
         <v>108</v>
       </c>
-      <c r="F74" s="214"/>
-      <c r="G74" s="215"/>
+      <c r="F74" s="215"/>
+      <c r="G74" s="214"/>
       <c r="H74" s="177"/>
       <c r="I74" s="175"/>
     </row>
@@ -23881,8 +23868,8 @@
       <c r="C75" s="172"/>
       <c r="D75" s="170"/>
       <c r="E75" s="195"/>
-      <c r="F75" s="215"/>
-      <c r="G75" s="215"/>
+      <c r="F75" s="214"/>
+      <c r="G75" s="214"/>
       <c r="H75" s="177"/>
       <c r="I75" s="175"/>
     </row>
@@ -23899,7 +23886,7 @@
         <v>[:lahtotiedot :jaahdytysjarjestelma :jaahdytyskauden-painotettu-kylmakerroin]</v>
       </c>
       <c r="F76" s="210"/>
-      <c r="G76" s="215"/>
+      <c r="G76" s="214"/>
       <c r="H76" s="177"/>
       <c r="I76" s="175"/>
       <c r="L76" s="193"/>
@@ -24972,8 +24959,8 @@
   </sheetPr>
   <dimension ref="A1:T113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F77" activeCellId="0" sqref="F77"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26347,9 +26334,9 @@
         <v>367</v>
       </c>
       <c r="E51" s="249"/>
-      <c r="F51" s="214"/>
-      <c r="G51" s="214"/>
-      <c r="H51" s="214"/>
+      <c r="F51" s="215"/>
+      <c r="G51" s="215"/>
+      <c r="H51" s="215"/>
       <c r="I51" s="180"/>
       <c r="J51" s="227"/>
       <c r="L51" s="233"/>
@@ -26457,7 +26444,7 @@
         <f aca="false">A96</f>
         <v>[:tulokset :nettotarve :tilojen-lammitys-vuosikulutus-nettoala]</v>
       </c>
-      <c r="H57" s="214"/>
+      <c r="H57" s="215"/>
       <c r="I57" s="182"/>
       <c r="J57" s="227"/>
     </row>
@@ -26478,7 +26465,7 @@
         <f aca="false">A98</f>
         <v>[:tulokset :nettotarve :ilmanvaihdon-lammitys-vuosikulutus-nettoala]</v>
       </c>
-      <c r="H58" s="215"/>
+      <c r="H58" s="214"/>
       <c r="I58" s="180"/>
       <c r="J58" s="228"/>
     </row>
@@ -26499,7 +26486,7 @@
         <f aca="false">A100</f>
         <v>[:tulokset :nettotarve :kayttoveden-valmistus-vuosikulutus-nettoala]</v>
       </c>
-      <c r="H59" s="214"/>
+      <c r="H59" s="215"/>
       <c r="I59" s="180"/>
       <c r="J59" s="227"/>
     </row>
@@ -26520,7 +26507,7 @@
         <f aca="false">A102</f>
         <v>[:tulokset :nettotarve :jaahdytys-vuosikulutus-nettoala]</v>
       </c>
-      <c r="H60" s="215"/>
+      <c r="H60" s="214"/>
       <c r="I60" s="180"/>
       <c r="J60" s="228"/>
     </row>
@@ -26653,7 +26640,7 @@
         <f aca="false">A104</f>
         <v>[:tulokset :lampokuormat :aurinko-nettoala]</v>
       </c>
-      <c r="H69" s="215"/>
+      <c r="H69" s="214"/>
       <c r="I69" s="182"/>
       <c r="J69" s="227"/>
     </row>
@@ -26674,7 +26661,7 @@
         <f aca="false">A106</f>
         <v>[:tulokset :lampokuormat :ihmiset-nettoala]</v>
       </c>
-      <c r="H70" s="215"/>
+      <c r="H70" s="214"/>
       <c r="I70" s="180"/>
       <c r="J70" s="228"/>
     </row>
@@ -26695,7 +26682,7 @@
         <f aca="false">A108</f>
         <v>[:tulokset :lampokuormat :kuluttajalaitteet-nettoala]</v>
       </c>
-      <c r="H71" s="215"/>
+      <c r="H71" s="214"/>
       <c r="I71" s="180"/>
       <c r="J71" s="227"/>
     </row>
@@ -26716,7 +26703,7 @@
         <f aca="false">A110</f>
         <v>[:tulokset :lampokuormat :valaistus-nettoala]</v>
       </c>
-      <c r="H72" s="215"/>
+      <c r="H72" s="214"/>
       <c r="I72" s="180"/>
       <c r="J72" s="227"/>
     </row>
@@ -26737,7 +26724,7 @@
         <f aca="false">A112</f>
         <v>[:tulokset :lampokuormat :kvesi-nettoala]</v>
       </c>
-      <c r="H73" s="215"/>
+      <c r="H73" s="214"/>
       <c r="I73" s="180"/>
       <c r="J73" s="228"/>
     </row>
@@ -27559,7 +27546,7 @@
   </sheetPr>
   <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -27568,8 +27555,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="90" width="61.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="0.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="1.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="23.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="26" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="26" width="7.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="26" width="15.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="7" style="26" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="26" width="2.42"/>

</xml_diff>

<commit_message>
Fix various xlsx template issues
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -4010,7 +4010,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="340">
+  <cellXfs count="341">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5365,6 +5365,10 @@
     </xf>
     <xf numFmtId="170" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -8979,9 +8983,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>246240</xdr:colOff>
+      <xdr:colOff>245880</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>259920</xdr:rowOff>
+      <xdr:rowOff>259560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8995,7 +8999,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="756000" cy="212400"/>
+          <a:ext cx="755640" cy="212040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9016,9 +9020,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>146160</xdr:colOff>
+      <xdr:colOff>145800</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>259920</xdr:rowOff>
+      <xdr:rowOff>259560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9032,7 +9036,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1099080" cy="212400"/>
+          <a:ext cx="1098720" cy="212040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9053,9 +9057,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>19440</xdr:colOff>
+      <xdr:colOff>19080</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>261000</xdr:rowOff>
+      <xdr:rowOff>260640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9069,7 +9073,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1406160" cy="212400"/>
+          <a:ext cx="1405800" cy="212040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9090,9 +9094,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>343440</xdr:colOff>
+      <xdr:colOff>343080</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>261000</xdr:rowOff>
+      <xdr:rowOff>260640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9106,7 +9110,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1730160" cy="212400"/>
+          <a:ext cx="1729800" cy="212040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9127,9 +9131,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>216720</xdr:colOff>
+      <xdr:colOff>216360</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>273960</xdr:rowOff>
+      <xdr:rowOff>273600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9143,7 +9147,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2037240" cy="225360"/>
+          <a:ext cx="2036880" cy="225000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9164,9 +9168,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>159840</xdr:colOff>
+      <xdr:colOff>159480</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>261000</xdr:rowOff>
+      <xdr:rowOff>260640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9180,7 +9184,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2382120" cy="212400"/>
+          <a:ext cx="2381760" cy="212040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9201,9 +9205,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>100080</xdr:colOff>
+      <xdr:colOff>99720</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>259920</xdr:rowOff>
+      <xdr:rowOff>259560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9217,7 +9221,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2695320" cy="212400"/>
+          <a:ext cx="2694960" cy="212040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9617,9 +9621,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>316440</xdr:colOff>
+      <xdr:colOff>316080</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>77400</xdr:rowOff>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9629,7 +9633,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="6998400" cy="10061640"/>
+          <a:ext cx="6998040" cy="10061280"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9715,9 +9719,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>4320</xdr:colOff>
+      <xdr:colOff>3960</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9727,7 +9731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7015680" cy="265320"/>
+          <a:ext cx="7015320" cy="264960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9781,9 +9785,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>432720</xdr:colOff>
+      <xdr:colOff>432360</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>55800</xdr:rowOff>
+      <xdr:rowOff>55440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9793,7 +9797,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="794520" cy="266400"/>
+          <a:ext cx="794160" cy="266040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9845,9 +9849,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>431640</xdr:colOff>
+      <xdr:colOff>431280</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>195480</xdr:rowOff>
+      <xdr:rowOff>195120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9857,7 +9861,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="794520" cy="266400"/>
+          <a:ext cx="794160" cy="266040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -24959,7 +24963,7 @@
   </sheetPr>
   <dimension ref="A1:T113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -27555,8 +27559,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="90" width="61.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="0.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="1.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="23.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="26" width="7.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="26" width="7.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="26" width="15.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="7" style="26" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="26" width="2.42"/>
@@ -30606,8 +30610,8 @@
   </sheetPr>
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C61" activeCellId="0" sqref="C61"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31344,7 +31348,7 @@
       <c r="F59" s="5"/>
       <c r="G59" s="155"/>
     </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="11.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="150"/>
       <c r="C60" s="300" t="s">
         <v>650</v>
@@ -31354,47 +31358,47 @@
       <c r="F60" s="300"/>
       <c r="G60" s="300"/>
     </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="150"/>
-      <c r="C61" s="325" t="str">
+      <c r="C61" s="339" t="str">
         <f aca="false">A44</f>
         <v>[:huomiot :lisatietoja-fi]</v>
       </c>
-      <c r="D61" s="325"/>
-      <c r="E61" s="325"/>
-      <c r="F61" s="325"/>
-      <c r="G61" s="325"/>
-    </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D61" s="339"/>
+      <c r="E61" s="339"/>
+      <c r="F61" s="339"/>
+      <c r="G61" s="339"/>
+    </row>
+    <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="150"/>
-      <c r="C62" s="325"/>
-      <c r="D62" s="325"/>
-      <c r="E62" s="325"/>
-      <c r="F62" s="325"/>
-      <c r="G62" s="325"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C62" s="339"/>
+      <c r="D62" s="339"/>
+      <c r="E62" s="339"/>
+      <c r="F62" s="339"/>
+      <c r="G62" s="339"/>
+    </row>
+    <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="150"/>
-      <c r="C63" s="325"/>
-      <c r="D63" s="325"/>
-      <c r="E63" s="325"/>
-      <c r="F63" s="325"/>
-      <c r="G63" s="325"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C63" s="339"/>
+      <c r="D63" s="339"/>
+      <c r="E63" s="339"/>
+      <c r="F63" s="339"/>
+      <c r="G63" s="339"/>
+    </row>
+    <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="150"/>
-      <c r="C64" s="325"/>
-      <c r="D64" s="325"/>
-      <c r="E64" s="325"/>
-      <c r="F64" s="325"/>
-      <c r="G64" s="325"/>
+      <c r="C64" s="339"/>
+      <c r="D64" s="339"/>
+      <c r="E64" s="339"/>
+      <c r="F64" s="339"/>
+      <c r="G64" s="339"/>
     </row>
     <row r="65" customFormat="false" ht="5.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C65" s="143"/>
-      <c r="D65" s="144"/>
-      <c r="E65" s="144"/>
-      <c r="F65" s="144"/>
-      <c r="G65" s="157"/>
+      <c r="C65" s="339"/>
+      <c r="D65" s="339"/>
+      <c r="E65" s="339"/>
+      <c r="F65" s="339"/>
+      <c r="G65" s="339"/>
     </row>
     <row r="66" customFormat="false" ht="4.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -31413,7 +31417,7 @@
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="C43:G57"/>
     <mergeCell ref="C60:G60"/>
-    <mergeCell ref="C61:G64"/>
+    <mergeCell ref="C61:G65"/>
   </mergeCells>
   <conditionalFormatting sqref="B15:D16 B13:C16 H13:AMJ17 B17 C45:C49 A65:AMJ1048576 A1:AMJ12 C42:G44 C57:G57 E59:AMJ59 A58:AMJ58 B59:B63 H60:AMJ64 C61:C63 B39:B57 H39:AMJ57 B19:B37 H19:AMJ37 C22:G22 C19:F21 D14">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="471">
@@ -31556,15 +31560,15 @@
       <c r="A2" s="150" t="s">
         <v>651</v>
       </c>
-      <c r="C2" s="339" t="s">
+      <c r="C2" s="340" t="s">
         <v>652</v>
       </c>
-      <c r="D2" s="339"/>
-      <c r="E2" s="339"/>
-      <c r="F2" s="339"/>
-      <c r="G2" s="339"/>
-      <c r="H2" s="339"/>
-      <c r="I2" s="339"/>
+      <c r="D2" s="340"/>
+      <c r="E2" s="340"/>
+      <c r="F2" s="340"/>
+      <c r="G2" s="340"/>
+      <c r="H2" s="340"/>
+      <c r="I2" s="340"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="319" t="s">

</xml_diff>

<commit_message>
AE-1143 fix voimassaolo date in 2013 finnish energiatodistus template
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -8963,9 +8963,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>243360</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:rowOff>257040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8979,7 +8979,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="753480" cy="209880"/>
+          <a:ext cx="753120" cy="209520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9000,9 +9000,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>143640</xdr:colOff>
+      <xdr:colOff>143280</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:rowOff>257040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9016,7 +9016,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1096560" cy="209880"/>
+          <a:ext cx="1096200" cy="209520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9037,9 +9037,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>16920</xdr:colOff>
+      <xdr:colOff>16560</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>258120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9053,7 +9053,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1403640" cy="209880"/>
+          <a:ext cx="1403280" cy="209520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9074,9 +9074,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>340920</xdr:colOff>
+      <xdr:colOff>340560</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>258120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9090,7 +9090,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1727640" cy="209880"/>
+          <a:ext cx="1727280" cy="209520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9111,9 +9111,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>214200</xdr:colOff>
+      <xdr:colOff>213840</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>271440</xdr:rowOff>
+      <xdr:rowOff>271080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9127,7 +9127,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2034720" cy="222840"/>
+          <a:ext cx="2034360" cy="222480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9148,9 +9148,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>157320</xdr:colOff>
+      <xdr:colOff>156960</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>258120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9164,7 +9164,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2379600" cy="209880"/>
+          <a:ext cx="2379240" cy="209520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9185,9 +9185,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>97560</xdr:colOff>
+      <xdr:colOff>97200</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:rowOff>257040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9201,7 +9201,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2692800" cy="209880"/>
+          <a:ext cx="2692440" cy="209520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9601,9 +9601,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>313920</xdr:colOff>
+      <xdr:colOff>313560</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9613,7 +9613,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="6995880" cy="10059120"/>
+          <a:ext cx="6995520" cy="10058760"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9699,9 +9699,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>1800</xdr:colOff>
+      <xdr:colOff>1440</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9711,7 +9711,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7013160" cy="262800"/>
+          <a:ext cx="7012800" cy="262440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9765,9 +9765,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>430200</xdr:colOff>
+      <xdr:colOff>429840</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>53280</xdr:rowOff>
+      <xdr:rowOff>52920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9777,7 +9777,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="792000" cy="263880"/>
+          <a:ext cx="791640" cy="263520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9829,9 +9829,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>429120</xdr:colOff>
+      <xdr:colOff>428760</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>192960</xdr:rowOff>
+      <xdr:rowOff>192600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9841,7 +9841,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="792000" cy="263880"/>
+          <a:ext cx="791640" cy="263520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9894,8 +9894,8 @@
   </sheetPr>
   <dimension ref="A1:AK262"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L49" activeCellId="0" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11751,8 +11751,8 @@
       <c r="J48" s="79"/>
       <c r="K48" s="74"/>
       <c r="L48" s="80" t="str">
-        <f aca="false">A22</f>
-        <v>#function[solita.etp.service.energiatodistus-pdf/fn--49544]</v>
+        <f aca="false">A23</f>
+        <v>#function[solita.etp.service.energiatodistus-pdf/fn--49547]</v>
       </c>
       <c r="M48" s="80"/>
       <c r="N48" s="80"/>
@@ -22482,7 +22482,7 @@
   </sheetPr>
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D58" activeCellId="0" sqref="D58"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
AE-1290 add missing vuosi / år word to column header in page 3 of pdf templates
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="791">
   <si>
     <t xml:space="preserve">[:id]</t>
   </si>
@@ -1386,9 +1386,6 @@
   </si>
   <si>
     <t xml:space="preserve">kpl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kWh</t>
   </si>
   <si>
     <t xml:space="preserve">[:lahtotiedot :lammitys :tilat-ja-iv :tuoton-hyotysuhde]</t>
@@ -8963,9 +8960,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>243360</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>257040</xdr:rowOff>
+      <xdr:rowOff>256680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8979,7 +8976,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="753120" cy="209520"/>
+          <a:ext cx="752760" cy="209160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9000,9 +8997,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>143280</xdr:colOff>
+      <xdr:colOff>142920</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>257040</xdr:rowOff>
+      <xdr:rowOff>256680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9016,7 +9013,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1096200" cy="209520"/>
+          <a:ext cx="1095840" cy="209160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9037,9 +9034,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>16560</xdr:colOff>
+      <xdr:colOff>16200</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>257760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9053,7 +9050,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1403280" cy="209520"/>
+          <a:ext cx="1402920" cy="209160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9074,9 +9071,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>340560</xdr:colOff>
+      <xdr:colOff>340200</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>257760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9090,7 +9087,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1727280" cy="209520"/>
+          <a:ext cx="1726920" cy="209160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9111,9 +9108,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>213840</xdr:colOff>
+      <xdr:colOff>213480</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>271080</xdr:rowOff>
+      <xdr:rowOff>270720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9127,7 +9124,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2034360" cy="222480"/>
+          <a:ext cx="2034000" cy="222120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9148,9 +9145,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>156960</xdr:colOff>
+      <xdr:colOff>156600</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>257760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9164,7 +9161,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2379240" cy="209520"/>
+          <a:ext cx="2378880" cy="209160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9185,9 +9182,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>97200</xdr:colOff>
+      <xdr:colOff>96840</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>257040</xdr:rowOff>
+      <xdr:rowOff>256680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9201,7 +9198,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2692440" cy="209520"/>
+          <a:ext cx="2692080" cy="209160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9601,9 +9598,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>313560</xdr:colOff>
+      <xdr:colOff>313200</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
+      <xdr:rowOff>74160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9613,7 +9610,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="6995520" cy="10058760"/>
+          <a:ext cx="6995160" cy="10058400"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9699,9 +9696,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:colOff>1080</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9711,7 +9708,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7012800" cy="262440"/>
+          <a:ext cx="7012440" cy="262080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9765,9 +9762,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>429840</xdr:colOff>
+      <xdr:colOff>429480</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9777,7 +9774,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="791640" cy="263520"/>
+          <a:ext cx="791280" cy="263160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9829,9 +9826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>428760</xdr:colOff>
+      <xdr:colOff>428400</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>192600</xdr:rowOff>
+      <xdr:rowOff>192240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9841,7 +9838,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="791640" cy="263520"/>
+          <a:ext cx="791280" cy="263160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9894,7 +9891,7 @@
   </sheetPr>
   <dimension ref="A1:AK262"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L49" activeCellId="0" sqref="L49"/>
     </sheetView>
   </sheetViews>
@@ -22482,8 +22479,8 @@
   </sheetPr>
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D58" activeCellId="0" sqref="D58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F69" activeCellId="0" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23663,7 +23660,7 @@
         <v>279</v>
       </c>
       <c r="F66" s="184" t="s">
-        <v>280</v>
+        <v>107</v>
       </c>
       <c r="G66" s="182"/>
       <c r="H66" s="179"/>
@@ -23683,11 +23680,11 @@
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="160" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C68" s="174"/>
       <c r="D68" s="175" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E68" s="214" t="str">
         <f aca="false">A76</f>
@@ -23703,11 +23700,11 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="160" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C69" s="174"/>
       <c r="D69" s="175" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E69" s="214" t="str">
         <f aca="false">A78</f>
@@ -23723,7 +23720,7 @@
     </row>
     <row r="70" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="160" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C70" s="174"/>
       <c r="D70" s="179"/>
@@ -23735,12 +23732,12 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="160" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B71" s="85"/>
       <c r="C71" s="168"/>
       <c r="D71" s="94" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E71" s="169"/>
       <c r="F71" s="169"/>
@@ -23750,7 +23747,7 @@
     </row>
     <row r="72" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="160" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C72" s="174"/>
       <c r="D72" s="179"/>
@@ -23762,12 +23759,12 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="160" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C73" s="174"/>
       <c r="D73" s="172"/>
       <c r="E73" s="215" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F73" s="216"/>
       <c r="G73" s="216"/>
@@ -23776,7 +23773,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="160" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C74" s="174"/>
       <c r="D74" s="172"/>
@@ -23790,7 +23787,7 @@
     </row>
     <row r="75" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="160" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C75" s="174"/>
       <c r="D75" s="172"/>
@@ -23802,11 +23799,11 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="160" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C76" s="174"/>
       <c r="D76" s="175" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E76" s="188" t="str">
         <f aca="false">A80</f>
@@ -23820,7 +23817,7 @@
     </row>
     <row r="77" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="160" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C77" s="174"/>
       <c r="D77" s="179"/>
@@ -23832,12 +23829,12 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="160" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B78" s="85"/>
       <c r="C78" s="168"/>
       <c r="D78" s="94" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E78" s="169"/>
       <c r="F78" s="169"/>
@@ -23847,7 +23844,7 @@
     </row>
     <row r="79" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="160" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C79" s="174"/>
       <c r="D79" s="179"/>
@@ -23859,15 +23856,15 @@
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="160" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C80" s="174"/>
       <c r="D80" s="179"/>
       <c r="E80" s="182" t="s">
+        <v>298</v>
+      </c>
+      <c r="F80" s="218" t="s">
         <v>299</v>
-      </c>
-      <c r="F80" s="218" t="s">
-        <v>300</v>
       </c>
       <c r="G80" s="179"/>
       <c r="H80" s="179"/>
@@ -23875,12 +23872,12 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="160" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C81" s="174"/>
       <c r="D81" s="172"/>
       <c r="E81" s="184" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F81" s="185" t="s">
         <v>108</v>
@@ -23892,7 +23889,7 @@
     </row>
     <row r="82" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="160" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C82" s="174"/>
       <c r="D82" s="172"/>
@@ -23904,11 +23901,11 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="160" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C83" s="174"/>
       <c r="D83" s="175" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E83" s="214" t="str">
         <f aca="false">A81</f>
@@ -23924,7 +23921,7 @@
     </row>
     <row r="84" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="160" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C84" s="174"/>
       <c r="D84" s="179"/>
@@ -23936,12 +23933,12 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="160" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B85" s="85"/>
       <c r="C85" s="168"/>
       <c r="D85" s="94" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E85" s="169"/>
       <c r="F85" s="169"/>
@@ -23951,7 +23948,7 @@
     </row>
     <row r="86" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="160" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C86" s="174"/>
       <c r="D86" s="179"/>
@@ -23963,27 +23960,27 @@
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="160" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C87" s="174"/>
       <c r="D87" s="172"/>
       <c r="E87" s="197" t="s">
+        <v>309</v>
+      </c>
+      <c r="F87" s="182" t="s">
         <v>310</v>
       </c>
-      <c r="F87" s="182" t="s">
+      <c r="G87" s="182" t="s">
         <v>311</v>
       </c>
-      <c r="G87" s="182" t="s">
+      <c r="H87" s="197" t="s">
         <v>312</v>
-      </c>
-      <c r="H87" s="197" t="s">
-        <v>313</v>
       </c>
       <c r="I87" s="177"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="160" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C88" s="174"/>
       <c r="D88" s="172"/>
@@ -23991,19 +23988,19 @@
         <v>109</v>
       </c>
       <c r="F88" s="184" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G88" s="184" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H88" s="185" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I88" s="177"/>
     </row>
     <row r="89" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="160" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C89" s="174"/>
       <c r="D89" s="172"/>
@@ -24015,7 +24012,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="160" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C90" s="174"/>
       <c r="D90" s="219"/>
@@ -24039,7 +24036,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="160" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C91" s="174"/>
       <c r="D91" s="219"/>
@@ -24063,7 +24060,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="160" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C92" s="174"/>
       <c r="D92" s="219"/>
@@ -24087,7 +24084,7 @@
     </row>
     <row r="93" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="160" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C93" s="220"/>
       <c r="D93" s="221"/>
@@ -24099,7 +24096,7 @@
     </row>
     <row r="94" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="160" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -24922,7 +24919,7 @@
       </c>
       <c r="C2" s="225"/>
       <c r="D2" s="165" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E2" s="226"/>
       <c r="F2" s="165"/>
@@ -25032,11 +25029,11 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="160" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C9" s="174"/>
       <c r="D9" s="234" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E9" s="28" t="str">
         <f aca="false">A5</f>
@@ -25063,7 +25060,7 @@
       </c>
       <c r="C10" s="174"/>
       <c r="D10" s="238" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E10" s="239" t="str">
         <f aca="false">A6</f>
@@ -25112,7 +25109,7 @@
       </c>
       <c r="C12" s="168"/>
       <c r="D12" s="94" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E12" s="169"/>
       <c r="F12" s="169"/>
@@ -25132,7 +25129,7 @@
     </row>
     <row r="13" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="160" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C13" s="174"/>
       <c r="D13" s="179"/>
@@ -25158,16 +25155,16 @@
       </c>
       <c r="C14" s="174"/>
       <c r="D14" s="240" t="s">
+        <v>327</v>
+      </c>
+      <c r="E14" s="182" t="s">
         <v>328</v>
       </c>
-      <c r="E14" s="182" t="s">
+      <c r="F14" s="182" t="s">
         <v>329</v>
       </c>
-      <c r="F14" s="182" t="s">
+      <c r="G14" s="197" t="s">
         <v>330</v>
-      </c>
-      <c r="G14" s="197" t="s">
-        <v>331</v>
       </c>
       <c r="H14" s="197"/>
       <c r="I14" s="182"/>
@@ -25189,13 +25186,13 @@
       <c r="C15" s="174"/>
       <c r="D15" s="173"/>
       <c r="E15" s="182" t="s">
+        <v>331</v>
+      </c>
+      <c r="F15" s="182" t="s">
         <v>332</v>
       </c>
-      <c r="F15" s="182" t="s">
+      <c r="G15" s="197" t="s">
         <v>333</v>
-      </c>
-      <c r="G15" s="197" t="s">
-        <v>334</v>
       </c>
       <c r="H15" s="197"/>
       <c r="I15" s="184"/>
@@ -25223,7 +25220,7 @@
         <v>109</v>
       </c>
       <c r="G16" s="243" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H16" s="244" t="s">
         <v>110</v>
@@ -25242,7 +25239,7 @@
     </row>
     <row r="17" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="160" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C17" s="174"/>
       <c r="D17" s="172"/>
@@ -25372,7 +25369,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="160" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C21" s="174"/>
       <c r="D21" s="248" t="s">
@@ -25518,7 +25515,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="160" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C25" s="174"/>
       <c r="D25" s="251" t="str">
@@ -25559,7 +25556,7 @@
       </c>
       <c r="C26" s="174"/>
       <c r="D26" s="252" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E26" s="253" t="str">
         <f aca="false">A42</f>
@@ -25614,7 +25611,7 @@
       </c>
       <c r="C28" s="168"/>
       <c r="D28" s="94" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E28" s="169"/>
       <c r="F28" s="169"/>
@@ -25657,7 +25654,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="160" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C30" s="174"/>
       <c r="D30" s="172"/>
@@ -25713,7 +25710,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="160" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C32" s="174"/>
       <c r="D32" s="255" t="str">
@@ -25744,7 +25741,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="160" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C33" s="174"/>
       <c r="D33" s="255" t="str">
@@ -25775,7 +25772,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="160" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C34" s="174"/>
       <c r="D34" s="255" t="str">
@@ -25806,7 +25803,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="160" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C35" s="174"/>
       <c r="D35" s="255" t="str">
@@ -25837,7 +25834,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="160" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C36" s="174"/>
       <c r="D36" s="255" t="str">
@@ -25868,7 +25865,7 @@
     </row>
     <row r="37" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="160" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C37" s="174"/>
       <c r="D37" s="179"/>
@@ -25890,11 +25887,11 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="160" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C38" s="168"/>
       <c r="D38" s="94" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E38" s="169"/>
       <c r="F38" s="169"/>
@@ -25914,7 +25911,7 @@
     </row>
     <row r="39" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="160" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C39" s="174"/>
       <c r="D39" s="179"/>
@@ -25936,19 +25933,19 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="160" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C40" s="174"/>
       <c r="D40" s="172"/>
       <c r="E40" s="172"/>
       <c r="F40" s="197" t="s">
+        <v>351</v>
+      </c>
+      <c r="G40" s="182" t="s">
         <v>352</v>
       </c>
-      <c r="G40" s="182" t="s">
+      <c r="H40" s="182" t="s">
         <v>353</v>
-      </c>
-      <c r="H40" s="182" t="s">
-        <v>354</v>
       </c>
       <c r="I40" s="182"/>
       <c r="J40" s="230"/>
@@ -25964,7 +25961,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="160" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C41" s="174"/>
       <c r="D41" s="172"/>
@@ -25992,7 +25989,7 @@
     </row>
     <row r="42" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="160" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C42" s="174"/>
       <c r="D42" s="172"/>
@@ -26014,7 +26011,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="160" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C43" s="174"/>
       <c r="D43" s="175" t="s">
@@ -26042,7 +26039,7 @@
       </c>
       <c r="C44" s="174"/>
       <c r="D44" s="175" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E44" s="175"/>
       <c r="F44" s="246" t="str">
@@ -26070,11 +26067,11 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="160" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C45" s="174"/>
       <c r="D45" s="175" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E45" s="175"/>
       <c r="F45" s="188" t="str">
@@ -26102,11 +26099,11 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="160" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C46" s="174"/>
       <c r="D46" s="175" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E46" s="175"/>
       <c r="F46" s="188" t="str">
@@ -26134,11 +26131,11 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="160" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C47" s="174"/>
       <c r="D47" s="175" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E47" s="175"/>
       <c r="F47" s="188" t="str">
@@ -26165,11 +26162,11 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="160" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C48" s="174"/>
       <c r="D48" s="175" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E48" s="175"/>
       <c r="F48" s="188" t="str">
@@ -26198,11 +26195,11 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="160" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C49" s="174"/>
       <c r="D49" s="175" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E49" s="175"/>
       <c r="F49" s="188" t="str">
@@ -26229,11 +26226,11 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="160" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C50" s="174"/>
       <c r="D50" s="252" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E50" s="252"/>
       <c r="F50" s="261" t="str">
@@ -26262,11 +26259,11 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="160" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C51" s="174"/>
       <c r="D51" s="262" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E51" s="252"/>
       <c r="F51" s="217"/>
@@ -26286,7 +26283,7 @@
     </row>
     <row r="52" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="160" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C52" s="174"/>
       <c r="D52" s="179"/>
@@ -26308,11 +26305,11 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="160" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C53" s="168"/>
       <c r="D53" s="94" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E53" s="169"/>
       <c r="F53" s="169"/>
@@ -26323,7 +26320,7 @@
     </row>
     <row r="54" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="160" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C54" s="174"/>
       <c r="D54" s="179"/>
@@ -26336,7 +26333,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="160" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C55" s="174"/>
       <c r="D55" s="172"/>
@@ -26352,7 +26349,7 @@
     </row>
     <row r="56" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="160" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C56" s="174"/>
       <c r="D56" s="172"/>
@@ -26364,11 +26361,11 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="160" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C57" s="174"/>
       <c r="D57" s="175" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E57" s="175"/>
       <c r="F57" s="214" t="str">
@@ -26385,11 +26382,11 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="160" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C58" s="174"/>
       <c r="D58" s="175" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E58" s="175"/>
       <c r="F58" s="214" t="str">
@@ -26406,7 +26403,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="160" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C59" s="174"/>
       <c r="D59" s="175" t="s">
@@ -26427,11 +26424,11 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="160" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C60" s="174"/>
       <c r="D60" s="175" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E60" s="175"/>
       <c r="F60" s="214" t="str">
@@ -26448,7 +26445,7 @@
     </row>
     <row r="61" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="160" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C61" s="174"/>
       <c r="D61" s="175"/>
@@ -26461,11 +26458,11 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="160" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C62" s="174"/>
       <c r="D62" s="213" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E62" s="213"/>
       <c r="F62" s="213"/>
@@ -26476,11 +26473,11 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="160" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C63" s="174"/>
       <c r="D63" s="213" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E63" s="213"/>
       <c r="F63" s="213"/>
@@ -26491,7 +26488,7 @@
     </row>
     <row r="64" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="160" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C64" s="174"/>
       <c r="D64" s="175"/>
@@ -26504,11 +26501,11 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="160" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C65" s="168"/>
       <c r="D65" s="94" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E65" s="169"/>
       <c r="F65" s="169"/>
@@ -26519,7 +26516,7 @@
     </row>
     <row r="66" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="160" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C66" s="174"/>
       <c r="D66" s="179"/>
@@ -26532,7 +26529,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="160" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C67" s="174"/>
       <c r="D67" s="172"/>
@@ -26548,7 +26545,7 @@
     </row>
     <row r="68" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="160" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C68" s="174"/>
       <c r="D68" s="172"/>
@@ -26560,11 +26557,11 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="160" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C69" s="174"/>
       <c r="D69" s="175" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E69" s="175"/>
       <c r="F69" s="214" t="str">
@@ -26581,11 +26578,11 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="160" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C70" s="174"/>
       <c r="D70" s="175" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E70" s="175"/>
       <c r="F70" s="214" t="str">
@@ -26602,11 +26599,11 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="160" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C71" s="174"/>
       <c r="D71" s="175" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E71" s="175"/>
       <c r="F71" s="214" t="str">
@@ -26623,11 +26620,11 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="160" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C72" s="174"/>
       <c r="D72" s="175" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E72" s="175"/>
       <c r="F72" s="214" t="str">
@@ -26644,11 +26641,11 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="160" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C73" s="174"/>
       <c r="D73" s="175" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E73" s="175"/>
       <c r="F73" s="214" t="str">
@@ -26665,7 +26662,7 @@
     </row>
     <row r="74" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="160" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C74" s="174"/>
       <c r="D74" s="175"/>
@@ -26678,11 +26675,11 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="160" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C75" s="168"/>
       <c r="D75" s="94" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E75" s="169"/>
       <c r="F75" s="169"/>
@@ -26693,7 +26690,7 @@
     </row>
     <row r="76" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="160" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C76" s="174"/>
       <c r="D76" s="179"/>
@@ -26706,11 +26703,11 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="160" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C77" s="174"/>
       <c r="D77" s="175" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E77" s="175"/>
       <c r="F77" s="263" t="str">
@@ -26724,7 +26721,7 @@
     </row>
     <row r="78" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="160" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C78" s="220"/>
       <c r="D78" s="221"/>
@@ -26737,177 +26734,177 @@
     </row>
     <row r="79" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="160" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="160" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="160" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="160" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="160" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="160" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="160" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="160" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="160" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="160" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="160" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="160" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="160" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="160" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="160" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="160" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="160" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="160" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="160" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="160" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="160" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="160" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="160" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="160" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="160" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="160" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="160" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="160" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="160" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="160" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="160" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="160" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="160" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="160" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="160" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -27510,7 +27507,7 @@
       </c>
       <c r="C2" s="266"/>
       <c r="D2" s="267" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E2" s="267"/>
       <c r="F2" s="267"/>
@@ -27527,7 +27524,7 @@
       </c>
       <c r="C3" s="97"/>
       <c r="D3" s="23" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E3" s="23"/>
       <c r="F3" s="270"/>
@@ -27540,7 +27537,7 @@
     </row>
     <row r="4" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="90" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C4" s="97"/>
       <c r="D4" s="14"/>
@@ -27555,11 +27552,11 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="90" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C5" s="93"/>
       <c r="D5" s="94" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E5" s="94"/>
       <c r="F5" s="94"/>
@@ -27572,7 +27569,7 @@
     </row>
     <row r="6" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="90" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C6" s="97"/>
       <c r="D6" s="14"/>
@@ -27587,7 +27584,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="90" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C7" s="97"/>
       <c r="D7" s="61" t="s">
@@ -27598,7 +27595,7 @@
         <v>[:lahtotiedot :lammitetty-nettoala]</v>
       </c>
       <c r="F7" s="271" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H7" s="272"/>
       <c r="K7" s="14"/>
@@ -27607,7 +27604,7 @@
     </row>
     <row r="8" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="90" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C8" s="97"/>
       <c r="D8" s="14"/>
@@ -27621,7 +27618,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="90" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C9" s="97"/>
       <c r="D9" s="14"/>
@@ -27636,11 +27633,11 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="90" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C10" s="97"/>
       <c r="D10" s="61" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E10" s="61"/>
       <c r="F10" s="14"/>
@@ -27657,7 +27654,7 @@
     </row>
     <row r="11" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="90" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C11" s="97"/>
       <c r="D11" s="14"/>
@@ -27672,11 +27669,11 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="90" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C12" s="97"/>
       <c r="D12" s="282" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E12" s="282"/>
       <c r="F12" s="282"/>
@@ -27696,11 +27693,11 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="90" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C13" s="97"/>
       <c r="D13" s="282" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E13" s="282"/>
       <c r="F13" s="282"/>
@@ -27720,11 +27717,11 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="90" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C14" s="97"/>
       <c r="D14" s="274" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E14" s="274"/>
       <c r="F14" s="282"/>
@@ -27744,11 +27741,11 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="90" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C15" s="97"/>
       <c r="D15" s="274" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E15" s="274"/>
       <c r="F15" s="282"/>
@@ -27768,11 +27765,11 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="90" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C16" s="97"/>
       <c r="D16" s="282" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E16" s="282"/>
       <c r="F16" s="282"/>
@@ -27792,7 +27789,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="90" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C17" s="97"/>
       <c r="D17" s="289" t="str">
@@ -27817,7 +27814,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="90" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C18" s="97"/>
       <c r="D18" s="289" t="str">
@@ -27842,7 +27839,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="90" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C19" s="97"/>
       <c r="D19" s="289" t="str">
@@ -27867,7 +27864,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="90" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C20" s="97"/>
       <c r="D20" s="289" t="str">
@@ -27892,7 +27889,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="90" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C21" s="97"/>
       <c r="D21" s="289" t="str">
@@ -27917,7 +27914,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="90" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C22" s="97"/>
       <c r="D22" s="290"/>
@@ -27936,7 +27933,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="90" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C23" s="97"/>
       <c r="D23" s="294"/>
@@ -27952,22 +27949,22 @@
     </row>
     <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="90" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C24" s="97"/>
       <c r="D24" s="297" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E24" s="297"/>
       <c r="F24" s="297"/>
       <c r="G24" s="298" t="s">
+        <v>473</v>
+      </c>
+      <c r="H24" s="299" t="s">
         <v>474</v>
       </c>
-      <c r="H24" s="299" t="s">
+      <c r="I24" s="298" t="s">
         <v>475</v>
-      </c>
-      <c r="I24" s="298" t="s">
-        <v>476</v>
       </c>
       <c r="J24" s="299" t="s">
         <v>107</v>
@@ -27980,7 +27977,7 @@
     </row>
     <row r="25" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="90" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C25" s="97"/>
       <c r="D25" s="61"/>
@@ -27996,11 +27993,11 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="90" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C26" s="97"/>
       <c r="D26" s="282" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E26" s="282"/>
       <c r="F26" s="282"/>
@@ -28009,7 +28006,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :kevyt-polttooljy]</v>
       </c>
       <c r="H26" s="303" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I26" s="276" t="n">
         <v>10</v>
@@ -28027,11 +28024,11 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="90" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C27" s="97"/>
       <c r="D27" s="282" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E27" s="282"/>
       <c r="F27" s="282"/>
@@ -28040,7 +28037,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :pilkkeet-havu-sekapuu]</v>
       </c>
       <c r="H27" s="303" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I27" s="276" t="n">
         <v>1300</v>
@@ -28058,11 +28055,11 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="90" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C28" s="97"/>
       <c r="D28" s="282" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E28" s="282"/>
       <c r="F28" s="282"/>
@@ -28071,7 +28068,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :pilkkeet-koivu]</v>
       </c>
       <c r="H28" s="303" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I28" s="276" t="n">
         <v>1700</v>
@@ -28089,11 +28086,11 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="90" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C29" s="97"/>
       <c r="D29" s="282" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E29" s="282"/>
       <c r="F29" s="282"/>
@@ -28102,7 +28099,7 @@
         <v>[:toteutunut-ostoenergiankulutus :ostetut-polttoaineet :puupelletit]</v>
       </c>
       <c r="H29" s="303" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I29" s="276" t="n">
         <v>4.7</v>
@@ -28120,7 +28117,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="90" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C30" s="97"/>
       <c r="D30" s="307" t="str">
@@ -28154,7 +28151,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="90" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C31" s="97"/>
       <c r="D31" s="307" t="str">
@@ -28188,7 +28185,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="90" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C32" s="97"/>
       <c r="D32" s="310"/>
@@ -28210,7 +28207,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="90" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C33" s="97"/>
       <c r="D33" s="310"/>
@@ -28232,7 +28229,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="90" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C34" s="97"/>
       <c r="D34" s="310"/>
@@ -28254,7 +28251,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="90" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C35" s="97"/>
       <c r="D35" s="310"/>
@@ -28276,7 +28273,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="90" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C36" s="97"/>
       <c r="D36" s="310"/>
@@ -28298,7 +28295,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="90" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C37" s="97"/>
       <c r="D37" s="310"/>
@@ -28320,7 +28317,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="90" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C38" s="97"/>
       <c r="D38" s="310"/>
@@ -28342,7 +28339,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="90" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C39" s="97"/>
       <c r="D39" s="310"/>
@@ -28364,7 +28361,7 @@
     </row>
     <row r="40" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="90" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C40" s="97"/>
       <c r="D40" s="294"/>
@@ -28380,11 +28377,11 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="90" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C41" s="97"/>
       <c r="D41" s="312" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E41" s="312"/>
       <c r="F41" s="294"/>
@@ -28398,7 +28395,7 @@
     </row>
     <row r="42" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="90" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C42" s="97"/>
       <c r="D42" s="313"/>
@@ -28414,7 +28411,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="90" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C43" s="97"/>
       <c r="D43" s="294"/>
@@ -28430,11 +28427,11 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="90" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C44" s="97"/>
       <c r="D44" s="61" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E44" s="61"/>
       <c r="F44" s="294"/>
@@ -28448,7 +28445,7 @@
     </row>
     <row r="45" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="90" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C45" s="97"/>
       <c r="D45" s="61"/>
@@ -28464,7 +28461,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="90" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C46" s="97"/>
       <c r="D46" s="61"/>
@@ -28484,11 +28481,11 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="90" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C47" s="97"/>
       <c r="D47" s="23" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E47" s="23"/>
       <c r="F47" s="23"/>
@@ -28508,11 +28505,11 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="90" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C48" s="97"/>
       <c r="D48" s="23" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E48" s="23"/>
       <c r="F48" s="23"/>
@@ -28532,11 +28529,11 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="90" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C49" s="97"/>
       <c r="D49" s="23" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E49" s="23"/>
       <c r="F49" s="23"/>
@@ -28556,11 +28553,11 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="90" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C50" s="97"/>
       <c r="D50" s="23" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E50" s="23"/>
       <c r="F50" s="23"/>
@@ -28580,11 +28577,11 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="90" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C51" s="97"/>
       <c r="D51" s="61" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E51" s="61"/>
       <c r="F51" s="61"/>
@@ -28603,7 +28600,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="90" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C52" s="97"/>
       <c r="D52" s="61"/>
@@ -28618,11 +28615,11 @@
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="90" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C53" s="97"/>
       <c r="D53" s="144" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E53" s="144"/>
       <c r="F53" s="144"/>
@@ -28635,7 +28632,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="90" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C54" s="97"/>
       <c r="D54" s="144"/>
@@ -28650,7 +28647,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="90" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C55" s="97"/>
       <c r="D55" s="144"/>
@@ -28665,7 +28662,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="90" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C56" s="97"/>
       <c r="D56" s="144"/>
@@ -28680,7 +28677,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="90" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C57" s="97"/>
       <c r="D57" s="144"/>
@@ -28695,7 +28692,7 @@
     </row>
     <row r="58" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="90" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C58" s="145"/>
       <c r="D58" s="146"/>
@@ -28711,47 +28708,47 @@
     </row>
     <row r="59" customFormat="false" ht="4.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="90" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="90" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="90" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="90" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="90" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="90" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="90" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="90" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="90" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
   </sheetData>
@@ -29463,10 +29460,10 @@
     </row>
     <row r="2" s="324" customFormat="true" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="323" t="s">
+        <v>532</v>
+      </c>
+      <c r="C2" s="325" t="s">
         <v>533</v>
-      </c>
-      <c r="C2" s="325" t="s">
-        <v>534</v>
       </c>
       <c r="D2" s="325"/>
       <c r="E2" s="325"/>
@@ -29475,7 +29472,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="152" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C3" s="326" t="s">
         <v>155</v>
@@ -29487,7 +29484,7 @@
     </row>
     <row r="4" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="322" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C4" s="145"/>
       <c r="D4" s="5"/>
@@ -29497,10 +29494,10 @@
     </row>
     <row r="5" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="322" t="s">
+        <v>536</v>
+      </c>
+      <c r="C5" s="327" t="s">
         <v>537</v>
-      </c>
-      <c r="C5" s="327" t="s">
-        <v>538</v>
       </c>
       <c r="D5" s="94"/>
       <c r="E5" s="169"/>
@@ -29509,7 +29506,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="322" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C6" s="328" t="str">
         <f aca="false">A2</f>
@@ -29522,7 +29519,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="322" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C7" s="328"/>
       <c r="D7" s="328"/>
@@ -29532,7 +29529,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="322" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C8" s="328"/>
       <c r="D8" s="328"/>
@@ -29542,7 +29539,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="322" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C9" s="328"/>
       <c r="D9" s="328"/>
@@ -29552,7 +29549,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="322" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C10" s="328"/>
       <c r="D10" s="328"/>
@@ -29562,7 +29559,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="322" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C11" s="328"/>
       <c r="D11" s="328"/>
@@ -29572,7 +29569,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="322" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C12" s="328"/>
       <c r="D12" s="328"/>
@@ -29582,7 +29579,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="322" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C13" s="328"/>
       <c r="D13" s="328"/>
@@ -29592,7 +29589,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="322" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C14" s="328"/>
       <c r="D14" s="328"/>
@@ -29602,7 +29599,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="322" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C15" s="328"/>
       <c r="D15" s="328"/>
@@ -29612,10 +29609,10 @@
     </row>
     <row r="16" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="152" t="s">
+        <v>548</v>
+      </c>
+      <c r="C16" s="329" t="s">
         <v>549</v>
-      </c>
-      <c r="C16" s="329" t="s">
-        <v>550</v>
       </c>
       <c r="D16" s="329"/>
       <c r="E16" s="329"/>
@@ -29624,7 +29621,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="152" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C17" s="330" t="n">
         <v>1</v>
@@ -29639,7 +29636,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="152" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C18" s="330" t="n">
         <v>2</v>
@@ -29654,7 +29651,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="152" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C19" s="330" t="n">
         <v>3</v>
@@ -29669,25 +29666,25 @@
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="152" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C20" s="332"/>
       <c r="D20" s="333" t="s">
+        <v>554</v>
+      </c>
+      <c r="E20" s="333" t="s">
         <v>555</v>
       </c>
-      <c r="E20" s="333" t="s">
+      <c r="F20" s="333" t="s">
         <v>556</v>
       </c>
-      <c r="F20" s="333" t="s">
+      <c r="G20" s="334" t="s">
         <v>557</v>
-      </c>
-      <c r="G20" s="334" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="152" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C21" s="332"/>
       <c r="D21" s="108" t="s">
@@ -29700,12 +29697,12 @@
         <v>107</v>
       </c>
       <c r="G21" s="108" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="152" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C22" s="330" t="n">
         <v>1</v>
@@ -29729,7 +29726,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="152" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C23" s="330" t="n">
         <v>2</v>
@@ -29753,7 +29750,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="152" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C24" s="330" t="n">
         <v>3</v>
@@ -29777,10 +29774,10 @@
     </row>
     <row r="25" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="152" t="s">
+        <v>563</v>
+      </c>
+      <c r="C25" s="336" t="s">
         <v>564</v>
-      </c>
-      <c r="C25" s="336" t="s">
-        <v>565</v>
       </c>
       <c r="D25" s="94"/>
       <c r="E25" s="169"/>
@@ -29789,7 +29786,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="152" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C26" s="328" t="str">
         <f aca="false">A22</f>
@@ -29802,7 +29799,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="152" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C27" s="328"/>
       <c r="D27" s="328"/>
@@ -29812,7 +29809,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="152" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C28" s="328"/>
       <c r="D28" s="328"/>
@@ -29822,7 +29819,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="152" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C29" s="328"/>
       <c r="D29" s="328"/>
@@ -29832,7 +29829,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="152" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C30" s="328"/>
       <c r="D30" s="328"/>
@@ -29842,7 +29839,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="152" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C31" s="328"/>
       <c r="D31" s="328"/>
@@ -29852,7 +29849,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="152" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C32" s="328"/>
       <c r="D32" s="328"/>
@@ -29862,7 +29859,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="152" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C33" s="328"/>
       <c r="D33" s="328"/>
@@ -29872,7 +29869,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="152" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C34" s="328"/>
       <c r="D34" s="328"/>
@@ -29882,7 +29879,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="152" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C35" s="328"/>
       <c r="D35" s="328"/>
@@ -29892,10 +29889,10 @@
     </row>
     <row r="36" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="152" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C36" s="329" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D36" s="329"/>
       <c r="E36" s="329"/>
@@ -29904,7 +29901,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="152" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C37" s="330" t="n">
         <v>1</v>
@@ -29919,7 +29916,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="152" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C38" s="330" t="n">
         <v>2</v>
@@ -29934,7 +29931,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="152" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C39" s="330" t="n">
         <v>3</v>
@@ -29949,25 +29946,25 @@
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="152" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C40" s="332"/>
       <c r="D40" s="333" t="s">
+        <v>554</v>
+      </c>
+      <c r="E40" s="333" t="s">
         <v>555</v>
       </c>
-      <c r="E40" s="333" t="s">
+      <c r="F40" s="333" t="s">
         <v>556</v>
       </c>
-      <c r="F40" s="333" t="s">
+      <c r="G40" s="334" t="s">
         <v>557</v>
-      </c>
-      <c r="G40" s="334" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="152" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C41" s="332"/>
       <c r="D41" s="108" t="s">
@@ -29980,12 +29977,12 @@
         <v>107</v>
       </c>
       <c r="G41" s="108" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="152" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C42" s="330" t="n">
         <v>1</v>
@@ -30009,7 +30006,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="152" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C43" s="330" t="n">
         <v>2</v>
@@ -30033,7 +30030,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="152" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C44" s="330" t="n">
         <v>3</v>
@@ -30057,10 +30054,10 @@
     </row>
     <row r="45" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="152" t="s">
+        <v>584</v>
+      </c>
+      <c r="C45" s="336" t="s">
         <v>585</v>
-      </c>
-      <c r="C45" s="336" t="s">
-        <v>586</v>
       </c>
       <c r="D45" s="338"/>
       <c r="E45" s="30"/>
@@ -30069,7 +30066,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="152" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C46" s="328" t="str">
         <f aca="false">A42</f>
@@ -30082,7 +30079,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="152" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C47" s="328"/>
       <c r="D47" s="328"/>
@@ -30092,7 +30089,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="152" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C48" s="328"/>
       <c r="D48" s="328"/>
@@ -30102,7 +30099,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="152" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C49" s="328"/>
       <c r="D49" s="328"/>
@@ -30112,7 +30109,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="152" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C50" s="328"/>
       <c r="D50" s="328"/>
@@ -30122,7 +30119,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="152" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C51" s="328"/>
       <c r="D51" s="328"/>
@@ -30132,7 +30129,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="152" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C52" s="328"/>
       <c r="D52" s="328"/>
@@ -30142,7 +30139,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="152" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C53" s="328"/>
       <c r="D53" s="328"/>
@@ -30152,7 +30149,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="152" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C54" s="328"/>
       <c r="D54" s="328"/>
@@ -30162,7 +30159,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="152" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C55" s="328"/>
       <c r="D55" s="328"/>
@@ -30172,10 +30169,10 @@
     </row>
     <row r="56" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="152" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C56" s="329" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D56" s="329"/>
       <c r="E56" s="329"/>
@@ -30184,7 +30181,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="152" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C57" s="330" t="n">
         <v>1</v>
@@ -30199,7 +30196,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="152" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C58" s="330" t="n">
         <v>2</v>
@@ -30214,7 +30211,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="152" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C59" s="330" t="n">
         <v>3</v>
@@ -30229,25 +30226,25 @@
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="152" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C60" s="332"/>
       <c r="D60" s="333" t="s">
+        <v>554</v>
+      </c>
+      <c r="E60" s="333" t="s">
         <v>555</v>
       </c>
-      <c r="E60" s="333" t="s">
+      <c r="F60" s="333" t="s">
         <v>556</v>
       </c>
-      <c r="F60" s="333" t="s">
+      <c r="G60" s="334" t="s">
         <v>557</v>
-      </c>
-      <c r="G60" s="334" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="152" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C61" s="332"/>
       <c r="D61" s="108" t="s">
@@ -30260,7 +30257,7 @@
         <v>107</v>
       </c>
       <c r="G61" s="108" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30563,10 +30560,10 @@
     </row>
     <row r="2" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="322" t="s">
+        <v>602</v>
+      </c>
+      <c r="C2" s="327" t="s">
         <v>603</v>
-      </c>
-      <c r="C2" s="327" t="s">
-        <v>604</v>
       </c>
       <c r="D2" s="94"/>
       <c r="E2" s="169"/>
@@ -30575,7 +30572,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="322" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C3" s="328" t="str">
         <f aca="false">A2</f>
@@ -30588,7 +30585,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="322" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C4" s="328"/>
       <c r="D4" s="328"/>
@@ -30598,7 +30595,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="322" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C5" s="328"/>
       <c r="D5" s="328"/>
@@ -30608,7 +30605,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="322" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C6" s="328"/>
       <c r="D6" s="328"/>
@@ -30618,7 +30615,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="322" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C7" s="328"/>
       <c r="D7" s="328"/>
@@ -30628,7 +30625,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="322" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C8" s="328"/>
       <c r="D8" s="328"/>
@@ -30638,7 +30635,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="322" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C9" s="328"/>
       <c r="D9" s="328"/>
@@ -30648,7 +30645,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="322" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C10" s="328"/>
       <c r="D10" s="328"/>
@@ -30658,7 +30655,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="322" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C11" s="328"/>
       <c r="D11" s="328"/>
@@ -30668,7 +30665,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="322" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C12" s="328"/>
       <c r="D12" s="328"/>
@@ -30678,10 +30675,10 @@
     </row>
     <row r="13" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="152" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C13" s="340" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D13" s="340"/>
       <c r="E13" s="340"/>
@@ -30690,7 +30687,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="152" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C14" s="330" t="n">
         <v>1</v>
@@ -30705,7 +30702,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="152" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C15" s="330" t="n">
         <v>2</v>
@@ -30720,7 +30717,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="152" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C16" s="330" t="n">
         <v>3</v>
@@ -30735,25 +30732,25 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="152" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C17" s="332"/>
       <c r="D17" s="333" t="s">
+        <v>554</v>
+      </c>
+      <c r="E17" s="333" t="s">
         <v>555</v>
       </c>
-      <c r="E17" s="333" t="s">
+      <c r="F17" s="333" t="s">
         <v>556</v>
       </c>
-      <c r="F17" s="333" t="s">
+      <c r="G17" s="334" t="s">
         <v>557</v>
-      </c>
-      <c r="G17" s="334" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="152" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C18" s="332"/>
       <c r="D18" s="108" t="s">
@@ -30766,12 +30763,12 @@
         <v>107</v>
       </c>
       <c r="G18" s="108" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="152" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C19" s="330" t="n">
         <v>1</v>
@@ -30795,7 +30792,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="152" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C20" s="330" t="n">
         <v>2</v>
@@ -30819,7 +30816,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="152" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C21" s="330" t="n">
         <v>3</v>
@@ -30843,10 +30840,10 @@
     </row>
     <row r="22" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="152" t="s">
+        <v>623</v>
+      </c>
+      <c r="C22" s="336" t="s">
         <v>624</v>
-      </c>
-      <c r="C22" s="336" t="s">
-        <v>625</v>
       </c>
       <c r="D22" s="338"/>
       <c r="E22" s="30"/>
@@ -30855,7 +30852,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="152" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C23" s="328" t="str">
         <f aca="false">A22</f>
@@ -30868,7 +30865,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="152" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C24" s="328"/>
       <c r="D24" s="328"/>
@@ -30878,7 +30875,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="152" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C25" s="328"/>
       <c r="D25" s="328"/>
@@ -30888,7 +30885,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="152" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C26" s="328"/>
       <c r="D26" s="328"/>
@@ -30898,7 +30895,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="152" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C27" s="328"/>
       <c r="D27" s="328"/>
@@ -30908,7 +30905,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="152" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C28" s="328"/>
       <c r="D28" s="328"/>
@@ -30918,7 +30915,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="152" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C29" s="328"/>
       <c r="D29" s="328"/>
@@ -30928,7 +30925,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="152" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C30" s="328"/>
       <c r="D30" s="328"/>
@@ -30938,7 +30935,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="152" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C31" s="328"/>
       <c r="D31" s="328"/>
@@ -30948,7 +30945,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="152" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C32" s="328"/>
       <c r="D32" s="328"/>
@@ -30958,10 +30955,10 @@
     </row>
     <row r="33" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="152" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C33" s="340" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D33" s="340"/>
       <c r="E33" s="340"/>
@@ -30970,7 +30967,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="152" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C34" s="330" t="n">
         <v>1</v>
@@ -30985,7 +30982,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="152" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C35" s="330" t="n">
         <v>2</v>
@@ -31000,7 +30997,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="152" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C36" s="330" t="n">
         <v>3</v>
@@ -31015,25 +31012,25 @@
     </row>
     <row r="37" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="152" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C37" s="332"/>
       <c r="D37" s="333" t="s">
+        <v>554</v>
+      </c>
+      <c r="E37" s="333" t="s">
         <v>555</v>
       </c>
-      <c r="E37" s="333" t="s">
+      <c r="F37" s="333" t="s">
         <v>556</v>
       </c>
-      <c r="F37" s="333" t="s">
+      <c r="G37" s="334" t="s">
         <v>557</v>
-      </c>
-      <c r="G37" s="334" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="152" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C38" s="332"/>
       <c r="D38" s="108" t="s">
@@ -31046,12 +31043,12 @@
         <v>107</v>
       </c>
       <c r="G38" s="108" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="152" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C39" s="330" t="n">
         <v>1</v>
@@ -31075,7 +31072,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="152" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C40" s="330" t="n">
         <v>2</v>
@@ -31099,7 +31096,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="152" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C41" s="330" t="n">
         <v>3</v>
@@ -31123,10 +31120,10 @@
     </row>
     <row r="42" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="152" t="s">
+        <v>644</v>
+      </c>
+      <c r="C42" s="336" t="s">
         <v>645</v>
-      </c>
-      <c r="C42" s="336" t="s">
-        <v>646</v>
       </c>
       <c r="D42" s="338"/>
       <c r="E42" s="30"/>
@@ -31135,7 +31132,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="152" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C43" s="328" t="str">
         <f aca="false">A42</f>
@@ -31148,7 +31145,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="152" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C44" s="328"/>
       <c r="D44" s="328"/>
@@ -31158,7 +31155,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="152" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C45" s="328"/>
       <c r="D45" s="328"/>
@@ -31264,7 +31261,7 @@
     </row>
     <row r="58" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C58" s="327" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D58" s="94"/>
       <c r="E58" s="169"/>
@@ -31282,7 +31279,7 @@
     <row r="60" customFormat="false" ht="11.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="152"/>
       <c r="C60" s="303" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D60" s="303"/>
       <c r="E60" s="303"/>
@@ -31489,10 +31486,10 @@
     </row>
     <row r="2" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="152" t="s">
+        <v>651</v>
+      </c>
+      <c r="C2" s="343" t="s">
         <v>652</v>
-      </c>
-      <c r="C2" s="343" t="s">
-        <v>653</v>
       </c>
       <c r="D2" s="343"/>
       <c r="E2" s="343"/>
@@ -31503,7 +31500,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="322" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C3" s="328" t="str">
         <f aca="false">A2</f>
@@ -31518,7 +31515,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="322" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C4" s="328"/>
       <c r="D4" s="328"/>
@@ -31530,7 +31527,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="322" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C5" s="328"/>
       <c r="D5" s="328"/>
@@ -31542,7 +31539,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="322" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C6" s="328"/>
       <c r="D6" s="328"/>
@@ -31554,7 +31551,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="322" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C7" s="328"/>
       <c r="D7" s="328"/>
@@ -31566,7 +31563,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="322" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C8" s="328"/>
       <c r="D8" s="328"/>
@@ -31578,7 +31575,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="322" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C9" s="328"/>
       <c r="D9" s="328"/>
@@ -31590,7 +31587,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="322" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C10" s="328"/>
       <c r="D10" s="328"/>
@@ -31602,7 +31599,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="322" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C11" s="328"/>
       <c r="D11" s="328"/>
@@ -31614,7 +31611,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="322" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C12" s="328"/>
       <c r="D12" s="328"/>
@@ -31626,7 +31623,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="322" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C13" s="328"/>
       <c r="D13" s="328"/>
@@ -31638,7 +31635,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="322" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C14" s="328"/>
       <c r="D14" s="328"/>
@@ -31650,7 +31647,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="322" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C15" s="328"/>
       <c r="D15" s="328"/>
@@ -31662,7 +31659,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="322" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C16" s="328"/>
       <c r="D16" s="328"/>
@@ -31674,7 +31671,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="322" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C17" s="328"/>
       <c r="D17" s="328"/>
@@ -31686,7 +31683,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="322" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C18" s="328"/>
       <c r="D18" s="328"/>
@@ -31698,7 +31695,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="322" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C19" s="328"/>
       <c r="D19" s="328"/>
@@ -31710,7 +31707,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="322" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C20" s="328"/>
       <c r="D20" s="328"/>
@@ -31722,7 +31719,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="322" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C21" s="328"/>
       <c r="D21" s="328"/>
@@ -31734,7 +31731,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="322" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C22" s="328"/>
       <c r="D22" s="328"/>
@@ -31746,7 +31743,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="322" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C23" s="328"/>
       <c r="D23" s="328"/>
@@ -31758,7 +31755,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="322" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C24" s="328"/>
       <c r="D24" s="328"/>
@@ -31770,7 +31767,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="322" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C25" s="328"/>
       <c r="D25" s="328"/>
@@ -31782,7 +31779,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="322" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C26" s="328"/>
       <c r="D26" s="328"/>
@@ -31794,7 +31791,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="322" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C27" s="328"/>
       <c r="D27" s="328"/>
@@ -31806,7 +31803,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="322" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C28" s="328"/>
       <c r="D28" s="328"/>
@@ -31818,7 +31815,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="322" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C29" s="328"/>
       <c r="D29" s="328"/>
@@ -31830,7 +31827,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="322" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C30" s="328"/>
       <c r="D30" s="328"/>
@@ -31842,7 +31839,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="322" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C31" s="328"/>
       <c r="D31" s="328"/>
@@ -31854,7 +31851,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="322" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C32" s="328"/>
       <c r="D32" s="328"/>
@@ -31866,7 +31863,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="322" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C33" s="328"/>
       <c r="D33" s="328"/>
@@ -31878,7 +31875,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="322" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C34" s="328"/>
       <c r="D34" s="328"/>
@@ -31890,7 +31887,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="322" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C35" s="328"/>
       <c r="D35" s="328"/>
@@ -31902,7 +31899,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="322" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C36" s="328"/>
       <c r="D36" s="328"/>
@@ -31914,7 +31911,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="322" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C37" s="328"/>
       <c r="D37" s="328"/>
@@ -31926,7 +31923,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="322" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C38" s="328"/>
       <c r="D38" s="328"/>
@@ -31938,7 +31935,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="322" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C39" s="328"/>
       <c r="D39" s="328"/>
@@ -31950,7 +31947,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="322" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C40" s="328"/>
       <c r="D40" s="328"/>
@@ -31962,7 +31959,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="322" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C41" s="328"/>
       <c r="D41" s="328"/>
@@ -31974,7 +31971,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="322" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C42" s="328"/>
       <c r="D42" s="328"/>
@@ -31986,7 +31983,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="322" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C43" s="328"/>
       <c r="D43" s="328"/>
@@ -31998,7 +31995,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="322" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C44" s="328"/>
       <c r="D44" s="328"/>
@@ -32010,7 +32007,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="322" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C45" s="328"/>
       <c r="D45" s="328"/>
@@ -32022,7 +32019,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="322" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C46" s="328"/>
       <c r="D46" s="328"/>
@@ -32034,7 +32031,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="322" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C47" s="328"/>
       <c r="D47" s="328"/>
@@ -32046,7 +32043,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="322" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C48" s="328"/>
       <c r="D48" s="328"/>
@@ -32058,7 +32055,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="322" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C49" s="328"/>
       <c r="D49" s="328"/>
@@ -32070,7 +32067,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="322" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C50" s="328"/>
       <c r="D50" s="328"/>
@@ -32082,7 +32079,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="322" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C51" s="328"/>
       <c r="D51" s="328"/>
@@ -32094,7 +32091,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="322" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C52" s="328"/>
       <c r="D52" s="328"/>
@@ -32106,7 +32103,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="322" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C53" s="328"/>
       <c r="D53" s="328"/>
@@ -32118,7 +32115,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="322" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C54" s="328"/>
       <c r="D54" s="328"/>
@@ -32130,7 +32127,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="322" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C55" s="328"/>
       <c r="D55" s="328"/>
@@ -32142,7 +32139,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="322" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C56" s="328"/>
       <c r="D56" s="328"/>
@@ -32154,7 +32151,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="322" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C57" s="328"/>
       <c r="D57" s="328"/>
@@ -32166,7 +32163,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="322" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C58" s="328"/>
       <c r="D58" s="328"/>
@@ -32178,7 +32175,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="322" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C59" s="328"/>
       <c r="D59" s="328"/>
@@ -32190,7 +32187,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="322" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C60" s="328"/>
       <c r="D60" s="328"/>
@@ -32202,7 +32199,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="322" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C61" s="328"/>
       <c r="D61" s="328"/>
@@ -32214,7 +32211,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="322" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C62" s="328"/>
       <c r="D62" s="328"/>
@@ -32226,7 +32223,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="322" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C63" s="328"/>
       <c r="D63" s="328"/>
@@ -32238,7 +32235,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="322" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C64" s="328"/>
       <c r="D64" s="328"/>
@@ -32250,7 +32247,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="322" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C65" s="328"/>
       <c r="D65" s="328"/>
@@ -32262,7 +32259,7 @@
     </row>
     <row r="66" customFormat="false" ht="5.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="322" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C66" s="145"/>
       <c r="D66" s="146"/>
@@ -32274,372 +32271,372 @@
     </row>
     <row r="67" customFormat="false" ht="4.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="322" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="322" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="322" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="322" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="322" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="322" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="322" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="322" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="322" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="322" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="322" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="322" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="322" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="322" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="322" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="322" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="322" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="322" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="322" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="322" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="322" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="322" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="322" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="322" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="322" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="322" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="322" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="322" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="322" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="322" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="322" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="322" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="322" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="322" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="322" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="322" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="322" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="322" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="322" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="322" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="322" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="322" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="322" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="322" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="322" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="322" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="322" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="322" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="322" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="322" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="322" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="322" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="322" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="322" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="322" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="322" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="322" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="322" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="322" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="322" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="322" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="322" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="322" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="322" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="322" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="322" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="322" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="322" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="322" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="322" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="322" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="322" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="322" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="322" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AE-528 Reorder energy sources on ET page 4
ET 2013
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -5003,7 +5003,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5011,7 +5011,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -8960,9 +8960,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>256680</xdr:rowOff>
+      <xdr:rowOff>256320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8976,12 +8976,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="752760" cy="209160"/>
+          <a:ext cx="752400" cy="208800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -8997,9 +8997,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>142920</xdr:colOff>
+      <xdr:colOff>142560</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>256680</xdr:rowOff>
+      <xdr:rowOff>256320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9013,12 +9013,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1095840" cy="209160"/>
+          <a:ext cx="1095480" cy="208800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -9034,9 +9034,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>16200</xdr:colOff>
+      <xdr:colOff>15840</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>257760</xdr:rowOff>
+      <xdr:rowOff>257400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9050,12 +9050,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1402920" cy="209160"/>
+          <a:ext cx="1402560" cy="208800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -9071,9 +9071,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>340200</xdr:colOff>
+      <xdr:colOff>339840</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>257760</xdr:rowOff>
+      <xdr:rowOff>257400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9087,12 +9087,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1726920" cy="209160"/>
+          <a:ext cx="1726560" cy="208800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -9108,9 +9108,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>213480</xdr:colOff>
+      <xdr:colOff>213120</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>270720</xdr:rowOff>
+      <xdr:rowOff>270360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9124,12 +9124,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2034000" cy="222120"/>
+          <a:ext cx="2033640" cy="221760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -9145,9 +9145,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>156600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>257760</xdr:rowOff>
+      <xdr:rowOff>257400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9161,12 +9161,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2378880" cy="209160"/>
+          <a:ext cx="2378520" cy="208800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -9182,9 +9182,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>96840</xdr:colOff>
+      <xdr:colOff>96480</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>256680</xdr:rowOff>
+      <xdr:rowOff>256320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9198,12 +9198,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2692080" cy="209160"/>
+          <a:ext cx="2691720" cy="208800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -9598,9 +9598,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>313200</xdr:colOff>
+      <xdr:colOff>312840</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>74160</xdr:rowOff>
+      <xdr:rowOff>73800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9610,7 +9610,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="6995160" cy="10058400"/>
+          <a:ext cx="6994800" cy="10058040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9695,10 +9695,10 @@
       <xdr:rowOff>128160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>1080</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>323280</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>75240</xdr:rowOff>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9708,7 +9708,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7012440" cy="262080"/>
+          <a:ext cx="7012080" cy="261720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9727,7 +9727,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000">
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -9745,7 +9745,7 @@
             </a:rPr>
             <a:t>Energiatodistus perustuu lakiin rakennuksen energiatodistuksesta (50/2013). </a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="fi-FI" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -9762,9 +9762,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>429480</xdr:colOff>
+      <xdr:colOff>429120</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9774,13 +9774,13 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="791280" cy="263160"/>
+          <a:ext cx="790920" cy="262800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -9809,7 +9809,7 @@
             </a:rPr>
             <a:t>Uudisrakennusten</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="700" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="fi-FI" sz="700" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -9826,9 +9826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>428400</xdr:colOff>
+      <xdr:colOff>428040</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>192240</xdr:rowOff>
+      <xdr:rowOff>191880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9838,13 +9838,13 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="791280" cy="263160"/>
+          <a:ext cx="790920" cy="262800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -9873,7 +9873,7 @@
             </a:rPr>
             <a:t>määräystaso 2012</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="700" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="fi-FI" sz="700" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -9891,8 +9891,8 @@
   </sheetPr>
   <dimension ref="A1:AK262"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L49" activeCellId="0" sqref="L49"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19679,18 +19679,18 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9:H11 J9:AMJ9 I10:AMJ11" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B9:H11 J9:AMJ9 I10:AMJ11" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A9:A11" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A9:A11" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -19707,7 +19707,7 @@
   <dimension ref="A1:AC82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22463,8 +22463,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -22479,8 +22479,8 @@
   </sheetPr>
   <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F69" activeCellId="0" sqref="F69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24869,14 +24869,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A49:E49 G49:AMJ49" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A49:E49 G49:AMJ49" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -24892,7 +24892,7 @@
   <dimension ref="A1:T113"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25337,23 +25337,23 @@
       </c>
       <c r="C20" s="174"/>
       <c r="D20" s="248" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E20" s="214" t="str">
-        <f aca="false">A15</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine]</v>
-      </c>
-      <c r="F20" s="246" t="str">
-        <f aca="false">A16</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine-kerroin]</v>
-      </c>
-      <c r="G20" s="214" t="str">
-        <f aca="false">A17</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine-kertoimella]</v>
-      </c>
-      <c r="H20" s="246" t="str">
-        <f aca="false">A18</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine-nettoala-kertoimella]</v>
+        <f aca="false">A23</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine]</v>
+      </c>
+      <c r="F20" s="249" t="str">
+        <f aca="false">A24</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine-kerroin]</v>
+      </c>
+      <c r="G20" s="247" t="str">
+        <f aca="false">A25</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine-kertoimella]</v>
+      </c>
+      <c r="H20" s="247" t="str">
+        <f aca="false">A26</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine-nettoala-kertoimella]</v>
       </c>
       <c r="I20" s="182"/>
       <c r="J20" s="230"/>
@@ -25372,24 +25372,24 @@
         <v>336</v>
       </c>
       <c r="C21" s="174"/>
-      <c r="D21" s="248" t="s">
-        <v>121</v>
+      <c r="D21" s="250" t="s">
+        <v>119</v>
       </c>
       <c r="E21" s="214" t="str">
-        <f aca="false">A19</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys]</v>
-      </c>
-      <c r="F21" s="249" t="str">
-        <f aca="false">A20</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys-kerroin]</v>
-      </c>
-      <c r="G21" s="247" t="str">
-        <f aca="false">A21</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys-kertoimella]</v>
-      </c>
-      <c r="H21" s="247" t="str">
-        <f aca="false">A22</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys-nettoala-kertoimella]</v>
+        <f aca="false">A15</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine]</v>
+      </c>
+      <c r="F21" s="246" t="str">
+        <f aca="false">A16</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine-kerroin]</v>
+      </c>
+      <c r="G21" s="214" t="str">
+        <f aca="false">A17</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine-kertoimella]</v>
+      </c>
+      <c r="H21" s="246" t="str">
+        <f aca="false">A18</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :fossiilinen-polttoaine-nettoala-kertoimella]</v>
       </c>
       <c r="I21" s="182"/>
       <c r="J21" s="229"/>
@@ -25409,23 +25409,23 @@
       </c>
       <c r="C22" s="174"/>
       <c r="D22" s="250" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E22" s="214" t="str">
-        <f aca="false">A23</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine]</v>
+        <f aca="false">A19</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys]</v>
       </c>
       <c r="F22" s="249" t="str">
-        <f aca="false">A24</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine-kerroin]</v>
+        <f aca="false">A20</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys-kerroin]</v>
       </c>
       <c r="G22" s="247" t="str">
-        <f aca="false">A25</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine-kertoimella]</v>
+        <f aca="false">A21</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys-kertoimella]</v>
       </c>
       <c r="H22" s="247" t="str">
-        <f aca="false">A26</f>
-        <v>[:tulokset :kaytettavat-energiamuodot :uusiutuva-polttoaine-nettoala-kertoimella]</v>
+        <f aca="false">A22</f>
+        <v>[:tulokset :kaytettavat-energiamuodot :kaukojaahdytys-nettoala-kertoimella]</v>
       </c>
       <c r="I22" s="182"/>
       <c r="J22" s="230"/>
@@ -25444,7 +25444,7 @@
         <v>118</v>
       </c>
       <c r="C23" s="174"/>
-      <c r="D23" s="250" t="str">
+      <c r="D23" s="248" t="str">
         <f aca="false">A27</f>
         <v>[:tulokset :kaytettavat-energiamuodot :muu 0 :nimi]</v>
       </c>
@@ -25481,7 +25481,7 @@
         <v>122</v>
       </c>
       <c r="C24" s="174"/>
-      <c r="D24" s="250" t="str">
+      <c r="D24" s="248" t="str">
         <f aca="false">A32</f>
         <v>[:tulokset :kaytettavat-energiamuodot :muu 1 :nimi]</v>
       </c>
@@ -27229,7 +27229,7 @@
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18:F25 H20">
+  <conditionalFormatting sqref="F18:F25 H22">
     <cfRule type="cellIs" priority="59" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="268">
       <formula>"*"</formula>
     </cfRule>
@@ -27269,12 +27269,12 @@
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G21:G25 G18:G19">
+  <conditionalFormatting sqref="G22:G25 G18:G20">
     <cfRule type="cellIs" priority="67" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="276">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21:H25 H18:H19">
+  <conditionalFormatting sqref="H22:H25 H18:H20">
     <cfRule type="cellIs" priority="68" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="277">
       <formula>"*"</formula>
     </cfRule>
@@ -27299,7 +27299,7 @@
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19:E25 G20">
+  <conditionalFormatting sqref="E19:E25 G22">
     <cfRule type="cellIs" priority="73" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="282">
       <formula>"*"</formula>
     </cfRule>
@@ -27407,9 +27407,9 @@
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D24">
+  <conditionalFormatting sqref="D23:D24 D20">
     <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148">
-      <formula>LEFT(D22,1)="*"</formula>
+      <formula>LEFT(D20,1)="*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:D19">
@@ -27417,53 +27417,53 @@
       <formula>"- Valitse -"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20:D21">
-    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183">
-      <formula>LEFT(D20,1)="*"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F44">
-    <cfRule type="cellIs" priority="98" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="302">
+    <cfRule type="cellIs" priority="97" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="302">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="cellIs" priority="99" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160">
+    <cfRule type="cellIs" priority="98" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47:H47 G49:H49">
-    <cfRule type="cellIs" priority="100" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161">
+    <cfRule type="cellIs" priority="99" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45:H46">
-    <cfRule type="cellIs" priority="101" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165">
+    <cfRule type="cellIs" priority="100" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D36">
-    <cfRule type="cellIs" priority="102" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186">
+    <cfRule type="cellIs" priority="101" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186">
       <formula>"tyhjä"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="103" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187">
+    <cfRule type="cellIs" priority="102" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D36">
-    <cfRule type="cellIs" priority="104" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188">
+    <cfRule type="cellIs" priority="103" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188">
       <formula>"- Valitse -"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D21:D22">
+    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183">
+      <formula>LEFT(D22,1)="*"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H44:H47 G47 G49:H49" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H44:H47 G47 G49:H49" type="none">
       <formula1>OR(ISNUMBER(#ref!),#ref!="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -27479,7 +27479,7 @@
   <dimension ref="A1:Z67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29422,8 +29422,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -29438,8 +29438,8 @@
   </sheetPr>
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K64" activeCellId="0" sqref="K64"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30516,14 +30516,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A63:F64 H63:AMJ64 G64" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A63:F64 H63:AMJ64 G64" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -30538,8 +30538,8 @@
   </sheetPr>
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31448,8 +31448,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -31465,7 +31465,7 @@
   <dimension ref="A1:I140"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32650,8 +32650,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
AE-1577 Update placeholders in ET templates
In the 8th page of each template:
- A9 to [:lahtotiedot :lammitys :lampohavio-lammittamaton-tila]
- A10 to UNUSED
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-2013-fi.xlsx
@@ -2977,10 +2977,10 @@
     <t xml:space="preserve">[:lahtotiedot :lammitys :lammin-kayttovesi :lampopumppu-tuotto-osuus]</t>
   </si>
   <si>
-    <t xml:space="preserve">[:lahtotiedot :lammitys :tilat-ja-iv :lampohavio-lammittamaton-tila]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:lahtotiedot :lammitys :lammin-kayttovesi :lampohavio-lammittamaton-tila]</t>
+    <t xml:space="preserve">[:lahtotiedot :lammitys :lampohavio-lammittamaton-tila]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNUSED</t>
   </si>
   <si>
     <t xml:space="preserve">[:tulokset :kuukausierittely 0 :tuotto :aurinkosahko]</t>
@@ -8960,9 +8960,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>242640</xdr:colOff>
+      <xdr:colOff>242280</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>256320</xdr:rowOff>
+      <xdr:rowOff>255960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8976,7 +8976,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4199040"/>
-          <a:ext cx="752400" cy="208800"/>
+          <a:ext cx="752040" cy="208440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8997,9 +8997,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>142560</xdr:colOff>
+      <xdr:colOff>142200</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>256320</xdr:rowOff>
+      <xdr:rowOff>255960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9013,7 +9013,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4513320"/>
-          <a:ext cx="1095480" cy="208800"/>
+          <a:ext cx="1095120" cy="208440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9034,9 +9034,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>15840</xdr:colOff>
+      <xdr:colOff>15480</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:rowOff>257040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9050,7 +9050,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="4828680"/>
-          <a:ext cx="1402560" cy="208800"/>
+          <a:ext cx="1402200" cy="208440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9071,9 +9071,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>339840</xdr:colOff>
+      <xdr:colOff>339480</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:rowOff>257040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9087,7 +9087,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5142960"/>
-          <a:ext cx="1726560" cy="208800"/>
+          <a:ext cx="1726200" cy="208440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9108,9 +9108,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>213120</xdr:colOff>
+      <xdr:colOff>212760</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>270360</xdr:rowOff>
+      <xdr:rowOff>270000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9124,7 +9124,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5457240"/>
-          <a:ext cx="2033640" cy="221760"/>
+          <a:ext cx="2033280" cy="221400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9145,9 +9145,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>156240</xdr:colOff>
+      <xdr:colOff>155880</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:rowOff>257040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9161,7 +9161,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="5771520"/>
-          <a:ext cx="2378520" cy="208800"/>
+          <a:ext cx="2378160" cy="208440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9182,9 +9182,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>96480</xdr:colOff>
+      <xdr:colOff>96120</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>256320</xdr:rowOff>
+      <xdr:rowOff>255960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9198,7 +9198,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3100680" y="6085080"/>
-          <a:ext cx="2691720" cy="208800"/>
+          <a:ext cx="2691360" cy="208440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9598,9 +9598,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>312840</xdr:colOff>
+      <xdr:colOff>312480</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:rowOff>73440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9610,7 +9610,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1994400" y="149040"/>
-          <a:ext cx="6994800" cy="10058040"/>
+          <a:ext cx="6994440" cy="10057680"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9696,9 +9696,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>323280</xdr:colOff>
+      <xdr:colOff>322920</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9708,7 +9708,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1987560" y="10344960"/>
-          <a:ext cx="7012080" cy="261720"/>
+          <a:ext cx="7011720" cy="261360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9762,9 +9762,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>429120</xdr:colOff>
+      <xdr:colOff>428760</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>52200</xdr:rowOff>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9774,7 +9774,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5525280" y="4883760"/>
-          <a:ext cx="790920" cy="262800"/>
+          <a:ext cx="790560" cy="262440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9826,9 +9826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>428040</xdr:colOff>
+      <xdr:colOff>427680</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>191880</xdr:rowOff>
+      <xdr:rowOff>191520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9838,7 +9838,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5524200" y="5023440"/>
-          <a:ext cx="790920" cy="262800"/>
+          <a:ext cx="790560" cy="262440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>